<commit_message>
Add second waffle chart
</commit_message>
<xml_diff>
--- a/data/Task1.xlsx
+++ b/data/Task1.xlsx
@@ -4,7 +4,8 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="events" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="nesting" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="level" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="favourite" sheetId="3" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -12,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="20">
   <si>
     <t>Participant ID</t>
   </si>
@@ -58,6 +59,21 @@
   <si>
     <t>Favourite overall</t>
   </si>
+  <si>
+    <t>Board A (level=2)</t>
+  </si>
+  <si>
+    <t>Board C (level=5)</t>
+  </si>
+  <si>
+    <t>Board B (level=3)</t>
+  </si>
+  <si>
+    <t>Personal (level=2)</t>
+  </si>
+  <si>
+    <t>Personal (level=4)</t>
+  </si>
 </sst>
 </file>
 
@@ -102,7 +118,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -139,6 +155,9 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="4" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -152,6 +171,10 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -12935,4 +12958,4118 @@
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="23.0"/>
+    <col customWidth="1" min="2" max="2" width="25.0"/>
+    <col customWidth="1" min="3" max="3" width="20.43"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="6">
+        <v>2.0</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="6">
+        <v>3.0</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="6">
+        <v>4.0</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="6">
+        <v>5.0</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="6">
+        <v>6.0</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="6">
+        <v>7.0</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="6">
+        <v>8.0</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="6">
+        <v>9.0</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="6">
+        <v>10.0</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="6">
+        <v>11.0</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="6">
+        <v>12.0</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="6">
+        <v>13.0</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="6">
+        <v>14.0</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="11"/>
+      <c r="B15" s="11"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="11"/>
+      <c r="B16" s="10"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="10"/>
+      <c r="B17" s="10"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="10"/>
+      <c r="B18" s="10"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="10"/>
+      <c r="B19" s="10"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="10"/>
+      <c r="B20" s="10"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="10"/>
+      <c r="B21" s="10"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="10"/>
+      <c r="B22" s="10"/>
+    </row>
+    <row r="23">
+      <c r="A23" s="10"/>
+      <c r="B23" s="10"/>
+    </row>
+    <row r="24">
+      <c r="A24" s="10"/>
+      <c r="B24" s="10"/>
+    </row>
+    <row r="25">
+      <c r="A25" s="10"/>
+      <c r="B25" s="10"/>
+    </row>
+    <row r="26">
+      <c r="A26" s="10"/>
+      <c r="B26" s="10"/>
+    </row>
+    <row r="27">
+      <c r="A27" s="10"/>
+      <c r="B27" s="10"/>
+    </row>
+    <row r="28">
+      <c r="A28" s="10"/>
+      <c r="B28" s="10"/>
+    </row>
+    <row r="29">
+      <c r="A29" s="10"/>
+      <c r="B29" s="10"/>
+    </row>
+    <row r="30">
+      <c r="A30" s="10"/>
+      <c r="B30" s="10"/>
+    </row>
+    <row r="31">
+      <c r="A31" s="10"/>
+      <c r="B31" s="10"/>
+    </row>
+    <row r="32">
+      <c r="A32" s="10"/>
+      <c r="B32" s="10"/>
+    </row>
+    <row r="33">
+      <c r="A33" s="10"/>
+      <c r="B33" s="10"/>
+    </row>
+    <row r="34">
+      <c r="A34" s="10"/>
+      <c r="B34" s="10"/>
+    </row>
+    <row r="35">
+      <c r="A35" s="10"/>
+      <c r="B35" s="10"/>
+    </row>
+    <row r="36">
+      <c r="A36" s="10"/>
+      <c r="B36" s="10"/>
+    </row>
+    <row r="37">
+      <c r="A37" s="10"/>
+      <c r="B37" s="10"/>
+    </row>
+    <row r="38">
+      <c r="A38" s="10"/>
+      <c r="B38" s="10"/>
+    </row>
+    <row r="39">
+      <c r="A39" s="3"/>
+      <c r="B39" s="3"/>
+    </row>
+    <row r="40">
+      <c r="A40" s="3"/>
+      <c r="B40" s="3"/>
+    </row>
+    <row r="41">
+      <c r="A41" s="3"/>
+      <c r="B41" s="3"/>
+    </row>
+    <row r="42">
+      <c r="A42" s="3"/>
+      <c r="B42" s="3"/>
+    </row>
+    <row r="43">
+      <c r="A43" s="3"/>
+      <c r="B43" s="3"/>
+    </row>
+    <row r="44">
+      <c r="A44" s="3"/>
+      <c r="B44" s="3"/>
+    </row>
+    <row r="45">
+      <c r="A45" s="3"/>
+      <c r="B45" s="3"/>
+    </row>
+    <row r="46">
+      <c r="A46" s="3"/>
+      <c r="B46" s="3"/>
+    </row>
+    <row r="47">
+      <c r="A47" s="3"/>
+      <c r="B47" s="3"/>
+    </row>
+    <row r="48">
+      <c r="A48" s="3"/>
+      <c r="B48" s="3"/>
+    </row>
+    <row r="49">
+      <c r="A49" s="3"/>
+      <c r="B49" s="3"/>
+    </row>
+    <row r="50">
+      <c r="A50" s="3"/>
+      <c r="B50" s="3"/>
+    </row>
+    <row r="51">
+      <c r="A51" s="3"/>
+      <c r="B51" s="3"/>
+    </row>
+    <row r="52">
+      <c r="A52" s="3"/>
+      <c r="B52" s="3"/>
+    </row>
+    <row r="53">
+      <c r="A53" s="3"/>
+      <c r="B53" s="3"/>
+    </row>
+    <row r="54">
+      <c r="A54" s="3"/>
+      <c r="B54" s="3"/>
+    </row>
+    <row r="55">
+      <c r="A55" s="3"/>
+      <c r="B55" s="3"/>
+    </row>
+    <row r="56">
+      <c r="A56" s="3"/>
+      <c r="B56" s="3"/>
+    </row>
+    <row r="57">
+      <c r="A57" s="3"/>
+      <c r="B57" s="3"/>
+    </row>
+    <row r="58">
+      <c r="A58" s="3"/>
+      <c r="B58" s="3"/>
+    </row>
+    <row r="59">
+      <c r="A59" s="3"/>
+      <c r="B59" s="3"/>
+    </row>
+    <row r="60">
+      <c r="A60" s="3"/>
+      <c r="B60" s="3"/>
+    </row>
+    <row r="61">
+      <c r="A61" s="3"/>
+      <c r="B61" s="3"/>
+    </row>
+    <row r="62">
+      <c r="A62" s="3"/>
+      <c r="B62" s="3"/>
+    </row>
+    <row r="63">
+      <c r="A63" s="3"/>
+      <c r="B63" s="3"/>
+    </row>
+    <row r="64">
+      <c r="A64" s="3"/>
+      <c r="B64" s="3"/>
+    </row>
+    <row r="65">
+      <c r="A65" s="3"/>
+      <c r="B65" s="3"/>
+    </row>
+    <row r="66">
+      <c r="A66" s="3"/>
+      <c r="B66" s="3"/>
+    </row>
+    <row r="67">
+      <c r="A67" s="3"/>
+      <c r="B67" s="3"/>
+    </row>
+    <row r="68">
+      <c r="A68" s="3"/>
+      <c r="B68" s="3"/>
+    </row>
+    <row r="69">
+      <c r="A69" s="3"/>
+      <c r="B69" s="3"/>
+    </row>
+    <row r="70">
+      <c r="A70" s="3"/>
+      <c r="B70" s="3"/>
+    </row>
+    <row r="71">
+      <c r="A71" s="3"/>
+      <c r="B71" s="3"/>
+    </row>
+    <row r="72">
+      <c r="A72" s="3"/>
+      <c r="B72" s="3"/>
+    </row>
+    <row r="73">
+      <c r="A73" s="3"/>
+      <c r="B73" s="3"/>
+    </row>
+    <row r="74">
+      <c r="A74" s="3"/>
+      <c r="B74" s="3"/>
+    </row>
+    <row r="75">
+      <c r="A75" s="3"/>
+      <c r="B75" s="3"/>
+    </row>
+    <row r="76">
+      <c r="A76" s="3"/>
+      <c r="B76" s="3"/>
+    </row>
+    <row r="77">
+      <c r="A77" s="3"/>
+      <c r="B77" s="3"/>
+    </row>
+    <row r="78">
+      <c r="A78" s="3"/>
+      <c r="B78" s="3"/>
+    </row>
+    <row r="79">
+      <c r="A79" s="3"/>
+      <c r="B79" s="3"/>
+    </row>
+    <row r="80">
+      <c r="A80" s="3"/>
+      <c r="B80" s="3"/>
+    </row>
+    <row r="81">
+      <c r="A81" s="3"/>
+      <c r="B81" s="3"/>
+    </row>
+    <row r="82">
+      <c r="A82" s="3"/>
+      <c r="B82" s="3"/>
+    </row>
+    <row r="83">
+      <c r="A83" s="3"/>
+      <c r="B83" s="3"/>
+    </row>
+    <row r="84">
+      <c r="A84" s="3"/>
+      <c r="B84" s="3"/>
+    </row>
+    <row r="85">
+      <c r="A85" s="3"/>
+      <c r="B85" s="3"/>
+    </row>
+    <row r="86">
+      <c r="A86" s="3"/>
+      <c r="B86" s="3"/>
+    </row>
+    <row r="87">
+      <c r="A87" s="3"/>
+      <c r="B87" s="3"/>
+    </row>
+    <row r="88">
+      <c r="A88" s="3"/>
+      <c r="B88" s="3"/>
+    </row>
+    <row r="89">
+      <c r="A89" s="3"/>
+      <c r="B89" s="3"/>
+    </row>
+    <row r="90">
+      <c r="A90" s="3"/>
+      <c r="B90" s="3"/>
+    </row>
+    <row r="91">
+      <c r="A91" s="3"/>
+      <c r="B91" s="3"/>
+    </row>
+    <row r="92">
+      <c r="A92" s="3"/>
+      <c r="B92" s="3"/>
+    </row>
+    <row r="93">
+      <c r="A93" s="3"/>
+      <c r="B93" s="3"/>
+    </row>
+    <row r="94">
+      <c r="A94" s="3"/>
+      <c r="B94" s="3"/>
+    </row>
+    <row r="95">
+      <c r="A95" s="3"/>
+      <c r="B95" s="3"/>
+    </row>
+    <row r="96">
+      <c r="A96" s="3"/>
+      <c r="B96" s="3"/>
+    </row>
+    <row r="97">
+      <c r="A97" s="3"/>
+      <c r="B97" s="3"/>
+    </row>
+    <row r="98">
+      <c r="A98" s="3"/>
+      <c r="B98" s="3"/>
+    </row>
+    <row r="99">
+      <c r="A99" s="3"/>
+      <c r="B99" s="3"/>
+    </row>
+    <row r="100">
+      <c r="A100" s="3"/>
+      <c r="B100" s="3"/>
+    </row>
+    <row r="101">
+      <c r="A101" s="3"/>
+      <c r="B101" s="3"/>
+    </row>
+    <row r="102">
+      <c r="A102" s="3"/>
+      <c r="B102" s="3"/>
+    </row>
+    <row r="103">
+      <c r="A103" s="3"/>
+      <c r="B103" s="3"/>
+    </row>
+    <row r="104">
+      <c r="A104" s="3"/>
+      <c r="B104" s="3"/>
+    </row>
+    <row r="105">
+      <c r="A105" s="3"/>
+      <c r="B105" s="3"/>
+    </row>
+    <row r="106">
+      <c r="A106" s="3"/>
+      <c r="B106" s="3"/>
+    </row>
+    <row r="107">
+      <c r="A107" s="3"/>
+      <c r="B107" s="3"/>
+    </row>
+    <row r="108">
+      <c r="A108" s="3"/>
+      <c r="B108" s="3"/>
+    </row>
+    <row r="109">
+      <c r="A109" s="3"/>
+      <c r="B109" s="3"/>
+    </row>
+    <row r="110">
+      <c r="A110" s="3"/>
+      <c r="B110" s="3"/>
+    </row>
+    <row r="111">
+      <c r="A111" s="3"/>
+      <c r="B111" s="3"/>
+    </row>
+    <row r="112">
+      <c r="A112" s="3"/>
+      <c r="B112" s="3"/>
+    </row>
+    <row r="113">
+      <c r="A113" s="3"/>
+      <c r="B113" s="3"/>
+    </row>
+    <row r="114">
+      <c r="A114" s="3"/>
+      <c r="B114" s="3"/>
+    </row>
+    <row r="115">
+      <c r="A115" s="3"/>
+      <c r="B115" s="3"/>
+    </row>
+    <row r="116">
+      <c r="A116" s="3"/>
+      <c r="B116" s="3"/>
+    </row>
+    <row r="117">
+      <c r="A117" s="3"/>
+      <c r="B117" s="3"/>
+    </row>
+    <row r="118">
+      <c r="A118" s="3"/>
+      <c r="B118" s="3"/>
+    </row>
+    <row r="119">
+      <c r="A119" s="3"/>
+      <c r="B119" s="3"/>
+    </row>
+    <row r="120">
+      <c r="A120" s="3"/>
+      <c r="B120" s="3"/>
+    </row>
+    <row r="121">
+      <c r="A121" s="3"/>
+      <c r="B121" s="3"/>
+    </row>
+    <row r="122">
+      <c r="A122" s="3"/>
+      <c r="B122" s="3"/>
+    </row>
+    <row r="123">
+      <c r="A123" s="3"/>
+      <c r="B123" s="3"/>
+    </row>
+    <row r="124">
+      <c r="A124" s="3"/>
+      <c r="B124" s="3"/>
+    </row>
+    <row r="125">
+      <c r="A125" s="3"/>
+      <c r="B125" s="3"/>
+    </row>
+    <row r="126">
+      <c r="A126" s="3"/>
+      <c r="B126" s="3"/>
+    </row>
+    <row r="127">
+      <c r="A127" s="3"/>
+      <c r="B127" s="3"/>
+    </row>
+    <row r="128">
+      <c r="A128" s="3"/>
+      <c r="B128" s="3"/>
+    </row>
+    <row r="129">
+      <c r="A129" s="3"/>
+      <c r="B129" s="3"/>
+    </row>
+    <row r="130">
+      <c r="A130" s="3"/>
+      <c r="B130" s="3"/>
+    </row>
+    <row r="131">
+      <c r="A131" s="3"/>
+      <c r="B131" s="3"/>
+    </row>
+    <row r="132">
+      <c r="A132" s="3"/>
+      <c r="B132" s="3"/>
+    </row>
+    <row r="133">
+      <c r="A133" s="3"/>
+      <c r="B133" s="3"/>
+    </row>
+    <row r="134">
+      <c r="A134" s="3"/>
+      <c r="B134" s="3"/>
+    </row>
+    <row r="135">
+      <c r="A135" s="3"/>
+      <c r="B135" s="3"/>
+    </row>
+    <row r="136">
+      <c r="A136" s="3"/>
+      <c r="B136" s="3"/>
+    </row>
+    <row r="137">
+      <c r="A137" s="3"/>
+      <c r="B137" s="3"/>
+    </row>
+    <row r="138">
+      <c r="A138" s="3"/>
+      <c r="B138" s="3"/>
+    </row>
+    <row r="139">
+      <c r="A139" s="3"/>
+      <c r="B139" s="3"/>
+    </row>
+    <row r="140">
+      <c r="A140" s="3"/>
+      <c r="B140" s="3"/>
+    </row>
+    <row r="141">
+      <c r="A141" s="3"/>
+      <c r="B141" s="3"/>
+    </row>
+    <row r="142">
+      <c r="A142" s="3"/>
+      <c r="B142" s="3"/>
+    </row>
+    <row r="143">
+      <c r="A143" s="3"/>
+      <c r="B143" s="3"/>
+    </row>
+    <row r="144">
+      <c r="A144" s="3"/>
+      <c r="B144" s="3"/>
+    </row>
+    <row r="145">
+      <c r="A145" s="3"/>
+      <c r="B145" s="3"/>
+    </row>
+    <row r="146">
+      <c r="A146" s="3"/>
+      <c r="B146" s="3"/>
+    </row>
+    <row r="147">
+      <c r="A147" s="3"/>
+      <c r="B147" s="3"/>
+    </row>
+    <row r="148">
+      <c r="A148" s="3"/>
+      <c r="B148" s="3"/>
+    </row>
+    <row r="149">
+      <c r="A149" s="3"/>
+      <c r="B149" s="3"/>
+    </row>
+    <row r="150">
+      <c r="A150" s="3"/>
+      <c r="B150" s="3"/>
+    </row>
+    <row r="151">
+      <c r="A151" s="3"/>
+      <c r="B151" s="3"/>
+    </row>
+    <row r="152">
+      <c r="A152" s="3"/>
+      <c r="B152" s="3"/>
+    </row>
+    <row r="153">
+      <c r="A153" s="3"/>
+      <c r="B153" s="3"/>
+    </row>
+    <row r="154">
+      <c r="A154" s="3"/>
+      <c r="B154" s="3"/>
+    </row>
+    <row r="155">
+      <c r="A155" s="3"/>
+      <c r="B155" s="3"/>
+    </row>
+    <row r="156">
+      <c r="A156" s="3"/>
+      <c r="B156" s="3"/>
+    </row>
+    <row r="157">
+      <c r="A157" s="3"/>
+      <c r="B157" s="3"/>
+    </row>
+    <row r="158">
+      <c r="A158" s="3"/>
+      <c r="B158" s="3"/>
+    </row>
+    <row r="159">
+      <c r="A159" s="3"/>
+      <c r="B159" s="3"/>
+    </row>
+    <row r="160">
+      <c r="A160" s="3"/>
+      <c r="B160" s="3"/>
+    </row>
+    <row r="161">
+      <c r="A161" s="3"/>
+      <c r="B161" s="3"/>
+    </row>
+    <row r="162">
+      <c r="A162" s="3"/>
+      <c r="B162" s="3"/>
+    </row>
+    <row r="163">
+      <c r="A163" s="3"/>
+      <c r="B163" s="3"/>
+    </row>
+    <row r="164">
+      <c r="A164" s="3"/>
+      <c r="B164" s="3"/>
+    </row>
+    <row r="165">
+      <c r="A165" s="3"/>
+      <c r="B165" s="3"/>
+    </row>
+    <row r="166">
+      <c r="A166" s="3"/>
+      <c r="B166" s="3"/>
+    </row>
+    <row r="167">
+      <c r="A167" s="3"/>
+      <c r="B167" s="3"/>
+    </row>
+    <row r="168">
+      <c r="A168" s="3"/>
+      <c r="B168" s="3"/>
+    </row>
+    <row r="169">
+      <c r="A169" s="3"/>
+      <c r="B169" s="3"/>
+    </row>
+    <row r="170">
+      <c r="A170" s="3"/>
+      <c r="B170" s="3"/>
+    </row>
+    <row r="171">
+      <c r="A171" s="3"/>
+      <c r="B171" s="3"/>
+    </row>
+    <row r="172">
+      <c r="A172" s="3"/>
+      <c r="B172" s="3"/>
+    </row>
+    <row r="173">
+      <c r="A173" s="3"/>
+      <c r="B173" s="3"/>
+    </row>
+    <row r="174">
+      <c r="A174" s="3"/>
+      <c r="B174" s="3"/>
+    </row>
+    <row r="175">
+      <c r="A175" s="3"/>
+      <c r="B175" s="3"/>
+    </row>
+    <row r="176">
+      <c r="A176" s="3"/>
+      <c r="B176" s="3"/>
+    </row>
+    <row r="177">
+      <c r="A177" s="3"/>
+      <c r="B177" s="3"/>
+    </row>
+    <row r="178">
+      <c r="A178" s="3"/>
+      <c r="B178" s="3"/>
+    </row>
+    <row r="179">
+      <c r="A179" s="3"/>
+      <c r="B179" s="3"/>
+    </row>
+    <row r="180">
+      <c r="A180" s="3"/>
+      <c r="B180" s="3"/>
+    </row>
+    <row r="181">
+      <c r="A181" s="3"/>
+      <c r="B181" s="3"/>
+    </row>
+    <row r="182">
+      <c r="A182" s="3"/>
+      <c r="B182" s="3"/>
+    </row>
+    <row r="183">
+      <c r="A183" s="3"/>
+      <c r="B183" s="3"/>
+    </row>
+    <row r="184">
+      <c r="A184" s="3"/>
+      <c r="B184" s="3"/>
+    </row>
+    <row r="185">
+      <c r="A185" s="3"/>
+      <c r="B185" s="3"/>
+    </row>
+    <row r="186">
+      <c r="A186" s="3"/>
+      <c r="B186" s="3"/>
+    </row>
+    <row r="187">
+      <c r="A187" s="3"/>
+      <c r="B187" s="3"/>
+    </row>
+    <row r="188">
+      <c r="A188" s="3"/>
+      <c r="B188" s="3"/>
+    </row>
+    <row r="189">
+      <c r="A189" s="3"/>
+      <c r="B189" s="3"/>
+    </row>
+    <row r="190">
+      <c r="A190" s="3"/>
+      <c r="B190" s="3"/>
+    </row>
+    <row r="191">
+      <c r="A191" s="3"/>
+      <c r="B191" s="3"/>
+    </row>
+    <row r="192">
+      <c r="A192" s="3"/>
+      <c r="B192" s="3"/>
+    </row>
+    <row r="193">
+      <c r="A193" s="3"/>
+      <c r="B193" s="3"/>
+    </row>
+    <row r="194">
+      <c r="A194" s="3"/>
+      <c r="B194" s="3"/>
+    </row>
+    <row r="195">
+      <c r="A195" s="3"/>
+      <c r="B195" s="3"/>
+    </row>
+    <row r="196">
+      <c r="A196" s="3"/>
+      <c r="B196" s="3"/>
+    </row>
+    <row r="197">
+      <c r="A197" s="3"/>
+      <c r="B197" s="3"/>
+    </row>
+    <row r="198">
+      <c r="A198" s="3"/>
+      <c r="B198" s="3"/>
+    </row>
+    <row r="199">
+      <c r="A199" s="3"/>
+      <c r="B199" s="3"/>
+    </row>
+    <row r="200">
+      <c r="A200" s="3"/>
+      <c r="B200" s="3"/>
+    </row>
+    <row r="201">
+      <c r="A201" s="3"/>
+      <c r="B201" s="3"/>
+    </row>
+    <row r="202">
+      <c r="A202" s="3"/>
+      <c r="B202" s="3"/>
+    </row>
+    <row r="203">
+      <c r="A203" s="3"/>
+      <c r="B203" s="3"/>
+    </row>
+    <row r="204">
+      <c r="A204" s="3"/>
+      <c r="B204" s="3"/>
+    </row>
+    <row r="205">
+      <c r="A205" s="3"/>
+      <c r="B205" s="3"/>
+    </row>
+    <row r="206">
+      <c r="A206" s="3"/>
+      <c r="B206" s="3"/>
+    </row>
+    <row r="207">
+      <c r="A207" s="3"/>
+      <c r="B207" s="3"/>
+    </row>
+    <row r="208">
+      <c r="A208" s="3"/>
+      <c r="B208" s="3"/>
+    </row>
+    <row r="209">
+      <c r="A209" s="3"/>
+      <c r="B209" s="3"/>
+    </row>
+    <row r="210">
+      <c r="A210" s="3"/>
+      <c r="B210" s="3"/>
+    </row>
+    <row r="211">
+      <c r="A211" s="3"/>
+      <c r="B211" s="3"/>
+    </row>
+    <row r="212">
+      <c r="A212" s="3"/>
+      <c r="B212" s="3"/>
+    </row>
+    <row r="213">
+      <c r="A213" s="3"/>
+      <c r="B213" s="3"/>
+    </row>
+    <row r="214">
+      <c r="A214" s="3"/>
+      <c r="B214" s="3"/>
+    </row>
+    <row r="215">
+      <c r="A215" s="3"/>
+      <c r="B215" s="3"/>
+    </row>
+    <row r="216">
+      <c r="A216" s="3"/>
+      <c r="B216" s="3"/>
+    </row>
+    <row r="217">
+      <c r="A217" s="3"/>
+      <c r="B217" s="3"/>
+    </row>
+    <row r="218">
+      <c r="A218" s="3"/>
+      <c r="B218" s="3"/>
+    </row>
+    <row r="219">
+      <c r="A219" s="3"/>
+      <c r="B219" s="3"/>
+    </row>
+    <row r="220">
+      <c r="A220" s="3"/>
+      <c r="B220" s="3"/>
+    </row>
+    <row r="221">
+      <c r="A221" s="3"/>
+      <c r="B221" s="3"/>
+    </row>
+    <row r="222">
+      <c r="A222" s="3"/>
+      <c r="B222" s="3"/>
+    </row>
+    <row r="223">
+      <c r="A223" s="3"/>
+      <c r="B223" s="3"/>
+    </row>
+    <row r="224">
+      <c r="A224" s="3"/>
+      <c r="B224" s="3"/>
+    </row>
+    <row r="225">
+      <c r="A225" s="3"/>
+      <c r="B225" s="3"/>
+    </row>
+    <row r="226">
+      <c r="A226" s="3"/>
+      <c r="B226" s="3"/>
+    </row>
+    <row r="227">
+      <c r="A227" s="3"/>
+      <c r="B227" s="3"/>
+    </row>
+    <row r="228">
+      <c r="A228" s="3"/>
+      <c r="B228" s="3"/>
+    </row>
+    <row r="229">
+      <c r="A229" s="3"/>
+      <c r="B229" s="3"/>
+    </row>
+    <row r="230">
+      <c r="A230" s="3"/>
+      <c r="B230" s="3"/>
+    </row>
+    <row r="231">
+      <c r="A231" s="3"/>
+      <c r="B231" s="3"/>
+    </row>
+    <row r="232">
+      <c r="A232" s="3"/>
+      <c r="B232" s="3"/>
+    </row>
+    <row r="233">
+      <c r="A233" s="3"/>
+      <c r="B233" s="3"/>
+    </row>
+    <row r="234">
+      <c r="A234" s="3"/>
+      <c r="B234" s="3"/>
+    </row>
+    <row r="235">
+      <c r="A235" s="3"/>
+      <c r="B235" s="3"/>
+    </row>
+    <row r="236">
+      <c r="A236" s="3"/>
+      <c r="B236" s="3"/>
+    </row>
+    <row r="237">
+      <c r="A237" s="3"/>
+      <c r="B237" s="3"/>
+    </row>
+    <row r="238">
+      <c r="A238" s="3"/>
+      <c r="B238" s="3"/>
+    </row>
+    <row r="239">
+      <c r="A239" s="3"/>
+      <c r="B239" s="3"/>
+    </row>
+    <row r="240">
+      <c r="A240" s="3"/>
+      <c r="B240" s="3"/>
+    </row>
+    <row r="241">
+      <c r="A241" s="3"/>
+      <c r="B241" s="3"/>
+    </row>
+    <row r="242">
+      <c r="A242" s="3"/>
+      <c r="B242" s="3"/>
+    </row>
+    <row r="243">
+      <c r="A243" s="3"/>
+      <c r="B243" s="3"/>
+    </row>
+    <row r="244">
+      <c r="A244" s="3"/>
+      <c r="B244" s="3"/>
+    </row>
+    <row r="245">
+      <c r="A245" s="3"/>
+      <c r="B245" s="3"/>
+    </row>
+    <row r="246">
+      <c r="A246" s="3"/>
+      <c r="B246" s="3"/>
+    </row>
+    <row r="247">
+      <c r="A247" s="3"/>
+      <c r="B247" s="3"/>
+    </row>
+    <row r="248">
+      <c r="A248" s="3"/>
+      <c r="B248" s="3"/>
+    </row>
+    <row r="249">
+      <c r="A249" s="3"/>
+      <c r="B249" s="3"/>
+    </row>
+    <row r="250">
+      <c r="A250" s="3"/>
+      <c r="B250" s="3"/>
+    </row>
+    <row r="251">
+      <c r="A251" s="3"/>
+      <c r="B251" s="3"/>
+    </row>
+    <row r="252">
+      <c r="A252" s="3"/>
+      <c r="B252" s="3"/>
+    </row>
+    <row r="253">
+      <c r="A253" s="3"/>
+      <c r="B253" s="3"/>
+    </row>
+    <row r="254">
+      <c r="A254" s="3"/>
+      <c r="B254" s="3"/>
+    </row>
+    <row r="255">
+      <c r="A255" s="3"/>
+      <c r="B255" s="3"/>
+    </row>
+    <row r="256">
+      <c r="A256" s="3"/>
+      <c r="B256" s="3"/>
+    </row>
+    <row r="257">
+      <c r="A257" s="3"/>
+      <c r="B257" s="3"/>
+    </row>
+    <row r="258">
+      <c r="A258" s="3"/>
+      <c r="B258" s="3"/>
+    </row>
+    <row r="259">
+      <c r="A259" s="3"/>
+      <c r="B259" s="3"/>
+    </row>
+    <row r="260">
+      <c r="A260" s="3"/>
+      <c r="B260" s="3"/>
+    </row>
+    <row r="261">
+      <c r="A261" s="3"/>
+      <c r="B261" s="3"/>
+    </row>
+    <row r="262">
+      <c r="A262" s="3"/>
+      <c r="B262" s="3"/>
+    </row>
+    <row r="263">
+      <c r="A263" s="3"/>
+      <c r="B263" s="3"/>
+    </row>
+    <row r="264">
+      <c r="A264" s="3"/>
+      <c r="B264" s="3"/>
+    </row>
+    <row r="265">
+      <c r="A265" s="3"/>
+      <c r="B265" s="3"/>
+    </row>
+    <row r="266">
+      <c r="A266" s="3"/>
+      <c r="B266" s="3"/>
+    </row>
+    <row r="267">
+      <c r="A267" s="3"/>
+      <c r="B267" s="3"/>
+    </row>
+    <row r="268">
+      <c r="A268" s="3"/>
+      <c r="B268" s="3"/>
+    </row>
+    <row r="269">
+      <c r="A269" s="3"/>
+      <c r="B269" s="3"/>
+    </row>
+    <row r="270">
+      <c r="A270" s="3"/>
+      <c r="B270" s="3"/>
+    </row>
+    <row r="271">
+      <c r="A271" s="3"/>
+      <c r="B271" s="3"/>
+    </row>
+    <row r="272">
+      <c r="A272" s="3"/>
+      <c r="B272" s="3"/>
+    </row>
+    <row r="273">
+      <c r="A273" s="3"/>
+      <c r="B273" s="3"/>
+    </row>
+    <row r="274">
+      <c r="A274" s="3"/>
+      <c r="B274" s="3"/>
+    </row>
+    <row r="275">
+      <c r="A275" s="3"/>
+      <c r="B275" s="3"/>
+    </row>
+    <row r="276">
+      <c r="A276" s="3"/>
+      <c r="B276" s="3"/>
+    </row>
+    <row r="277">
+      <c r="A277" s="3"/>
+      <c r="B277" s="3"/>
+    </row>
+    <row r="278">
+      <c r="A278" s="3"/>
+      <c r="B278" s="3"/>
+    </row>
+    <row r="279">
+      <c r="A279" s="3"/>
+      <c r="B279" s="3"/>
+    </row>
+    <row r="280">
+      <c r="A280" s="3"/>
+      <c r="B280" s="3"/>
+    </row>
+    <row r="281">
+      <c r="A281" s="3"/>
+      <c r="B281" s="3"/>
+    </row>
+    <row r="282">
+      <c r="A282" s="3"/>
+      <c r="B282" s="3"/>
+    </row>
+    <row r="283">
+      <c r="A283" s="3"/>
+      <c r="B283" s="3"/>
+    </row>
+    <row r="284">
+      <c r="A284" s="3"/>
+      <c r="B284" s="3"/>
+    </row>
+    <row r="285">
+      <c r="A285" s="3"/>
+      <c r="B285" s="3"/>
+    </row>
+    <row r="286">
+      <c r="A286" s="3"/>
+      <c r="B286" s="3"/>
+    </row>
+    <row r="287">
+      <c r="A287" s="3"/>
+      <c r="B287" s="3"/>
+    </row>
+    <row r="288">
+      <c r="A288" s="3"/>
+      <c r="B288" s="3"/>
+    </row>
+    <row r="289">
+      <c r="A289" s="3"/>
+      <c r="B289" s="3"/>
+    </row>
+    <row r="290">
+      <c r="A290" s="3"/>
+      <c r="B290" s="3"/>
+    </row>
+    <row r="291">
+      <c r="A291" s="3"/>
+      <c r="B291" s="3"/>
+    </row>
+    <row r="292">
+      <c r="A292" s="3"/>
+      <c r="B292" s="3"/>
+    </row>
+    <row r="293">
+      <c r="A293" s="3"/>
+      <c r="B293" s="3"/>
+    </row>
+    <row r="294">
+      <c r="A294" s="3"/>
+      <c r="B294" s="3"/>
+    </row>
+    <row r="295">
+      <c r="A295" s="3"/>
+      <c r="B295" s="3"/>
+    </row>
+    <row r="296">
+      <c r="A296" s="3"/>
+      <c r="B296" s="3"/>
+    </row>
+    <row r="297">
+      <c r="A297" s="3"/>
+      <c r="B297" s="3"/>
+    </row>
+    <row r="298">
+      <c r="A298" s="3"/>
+      <c r="B298" s="3"/>
+    </row>
+    <row r="299">
+      <c r="A299" s="3"/>
+      <c r="B299" s="3"/>
+    </row>
+    <row r="300">
+      <c r="A300" s="3"/>
+      <c r="B300" s="3"/>
+    </row>
+    <row r="301">
+      <c r="A301" s="3"/>
+      <c r="B301" s="3"/>
+    </row>
+    <row r="302">
+      <c r="A302" s="3"/>
+      <c r="B302" s="3"/>
+    </row>
+    <row r="303">
+      <c r="A303" s="3"/>
+      <c r="B303" s="3"/>
+    </row>
+    <row r="304">
+      <c r="A304" s="3"/>
+      <c r="B304" s="3"/>
+    </row>
+    <row r="305">
+      <c r="A305" s="3"/>
+      <c r="B305" s="3"/>
+    </row>
+    <row r="306">
+      <c r="A306" s="3"/>
+      <c r="B306" s="3"/>
+    </row>
+    <row r="307">
+      <c r="A307" s="3"/>
+      <c r="B307" s="3"/>
+    </row>
+    <row r="308">
+      <c r="A308" s="3"/>
+      <c r="B308" s="3"/>
+    </row>
+    <row r="309">
+      <c r="A309" s="3"/>
+      <c r="B309" s="3"/>
+    </row>
+    <row r="310">
+      <c r="A310" s="3"/>
+      <c r="B310" s="3"/>
+    </row>
+    <row r="311">
+      <c r="A311" s="3"/>
+      <c r="B311" s="3"/>
+    </row>
+    <row r="312">
+      <c r="A312" s="3"/>
+      <c r="B312" s="3"/>
+    </row>
+    <row r="313">
+      <c r="A313" s="3"/>
+      <c r="B313" s="3"/>
+    </row>
+    <row r="314">
+      <c r="A314" s="3"/>
+      <c r="B314" s="3"/>
+    </row>
+    <row r="315">
+      <c r="A315" s="3"/>
+      <c r="B315" s="3"/>
+    </row>
+    <row r="316">
+      <c r="A316" s="3"/>
+      <c r="B316" s="3"/>
+    </row>
+    <row r="317">
+      <c r="A317" s="3"/>
+      <c r="B317" s="3"/>
+    </row>
+    <row r="318">
+      <c r="A318" s="3"/>
+      <c r="B318" s="3"/>
+    </row>
+    <row r="319">
+      <c r="A319" s="3"/>
+      <c r="B319" s="3"/>
+    </row>
+    <row r="320">
+      <c r="A320" s="3"/>
+      <c r="B320" s="3"/>
+    </row>
+    <row r="321">
+      <c r="A321" s="3"/>
+      <c r="B321" s="3"/>
+    </row>
+    <row r="322">
+      <c r="A322" s="3"/>
+      <c r="B322" s="3"/>
+    </row>
+    <row r="323">
+      <c r="A323" s="3"/>
+      <c r="B323" s="3"/>
+    </row>
+    <row r="324">
+      <c r="A324" s="3"/>
+      <c r="B324" s="3"/>
+    </row>
+    <row r="325">
+      <c r="A325" s="3"/>
+      <c r="B325" s="3"/>
+    </row>
+    <row r="326">
+      <c r="A326" s="3"/>
+      <c r="B326" s="3"/>
+    </row>
+    <row r="327">
+      <c r="A327" s="3"/>
+      <c r="B327" s="3"/>
+    </row>
+    <row r="328">
+      <c r="A328" s="3"/>
+      <c r="B328" s="3"/>
+    </row>
+    <row r="329">
+      <c r="A329" s="3"/>
+      <c r="B329" s="3"/>
+    </row>
+    <row r="330">
+      <c r="A330" s="3"/>
+      <c r="B330" s="3"/>
+    </row>
+    <row r="331">
+      <c r="A331" s="3"/>
+      <c r="B331" s="3"/>
+    </row>
+    <row r="332">
+      <c r="A332" s="3"/>
+      <c r="B332" s="3"/>
+    </row>
+    <row r="333">
+      <c r="A333" s="3"/>
+      <c r="B333" s="3"/>
+    </row>
+    <row r="334">
+      <c r="A334" s="3"/>
+      <c r="B334" s="3"/>
+    </row>
+    <row r="335">
+      <c r="A335" s="3"/>
+      <c r="B335" s="3"/>
+    </row>
+    <row r="336">
+      <c r="A336" s="3"/>
+      <c r="B336" s="3"/>
+    </row>
+    <row r="337">
+      <c r="A337" s="3"/>
+      <c r="B337" s="3"/>
+    </row>
+    <row r="338">
+      <c r="A338" s="3"/>
+      <c r="B338" s="3"/>
+    </row>
+    <row r="339">
+      <c r="A339" s="3"/>
+      <c r="B339" s="3"/>
+    </row>
+    <row r="340">
+      <c r="A340" s="3"/>
+      <c r="B340" s="3"/>
+    </row>
+    <row r="341">
+      <c r="A341" s="3"/>
+      <c r="B341" s="3"/>
+    </row>
+    <row r="342">
+      <c r="A342" s="3"/>
+      <c r="B342" s="3"/>
+    </row>
+    <row r="343">
+      <c r="A343" s="3"/>
+      <c r="B343" s="3"/>
+    </row>
+    <row r="344">
+      <c r="A344" s="3"/>
+      <c r="B344" s="3"/>
+    </row>
+    <row r="345">
+      <c r="A345" s="3"/>
+      <c r="B345" s="3"/>
+    </row>
+    <row r="346">
+      <c r="A346" s="3"/>
+      <c r="B346" s="3"/>
+    </row>
+    <row r="347">
+      <c r="A347" s="3"/>
+      <c r="B347" s="3"/>
+    </row>
+    <row r="348">
+      <c r="A348" s="3"/>
+      <c r="B348" s="3"/>
+    </row>
+    <row r="349">
+      <c r="A349" s="3"/>
+      <c r="B349" s="3"/>
+    </row>
+    <row r="350">
+      <c r="A350" s="3"/>
+      <c r="B350" s="3"/>
+    </row>
+    <row r="351">
+      <c r="A351" s="3"/>
+      <c r="B351" s="3"/>
+    </row>
+    <row r="352">
+      <c r="A352" s="3"/>
+      <c r="B352" s="3"/>
+    </row>
+    <row r="353">
+      <c r="A353" s="3"/>
+      <c r="B353" s="3"/>
+    </row>
+    <row r="354">
+      <c r="A354" s="3"/>
+      <c r="B354" s="3"/>
+    </row>
+    <row r="355">
+      <c r="A355" s="3"/>
+      <c r="B355" s="3"/>
+    </row>
+    <row r="356">
+      <c r="A356" s="3"/>
+      <c r="B356" s="3"/>
+    </row>
+    <row r="357">
+      <c r="A357" s="3"/>
+      <c r="B357" s="3"/>
+    </row>
+    <row r="358">
+      <c r="A358" s="3"/>
+      <c r="B358" s="3"/>
+    </row>
+    <row r="359">
+      <c r="A359" s="3"/>
+      <c r="B359" s="3"/>
+    </row>
+    <row r="360">
+      <c r="A360" s="3"/>
+      <c r="B360" s="3"/>
+    </row>
+    <row r="361">
+      <c r="A361" s="3"/>
+      <c r="B361" s="3"/>
+    </row>
+    <row r="362">
+      <c r="A362" s="3"/>
+      <c r="B362" s="3"/>
+    </row>
+    <row r="363">
+      <c r="A363" s="3"/>
+      <c r="B363" s="3"/>
+    </row>
+    <row r="364">
+      <c r="A364" s="3"/>
+      <c r="B364" s="3"/>
+    </row>
+    <row r="365">
+      <c r="A365" s="3"/>
+      <c r="B365" s="3"/>
+    </row>
+    <row r="366">
+      <c r="A366" s="3"/>
+      <c r="B366" s="3"/>
+    </row>
+    <row r="367">
+      <c r="A367" s="3"/>
+      <c r="B367" s="3"/>
+    </row>
+    <row r="368">
+      <c r="A368" s="3"/>
+      <c r="B368" s="3"/>
+    </row>
+    <row r="369">
+      <c r="A369" s="3"/>
+      <c r="B369" s="3"/>
+    </row>
+    <row r="370">
+      <c r="A370" s="3"/>
+      <c r="B370" s="3"/>
+    </row>
+    <row r="371">
+      <c r="A371" s="3"/>
+      <c r="B371" s="3"/>
+    </row>
+    <row r="372">
+      <c r="A372" s="3"/>
+      <c r="B372" s="3"/>
+    </row>
+    <row r="373">
+      <c r="A373" s="3"/>
+      <c r="B373" s="3"/>
+    </row>
+    <row r="374">
+      <c r="A374" s="3"/>
+      <c r="B374" s="3"/>
+    </row>
+    <row r="375">
+      <c r="A375" s="3"/>
+      <c r="B375" s="3"/>
+    </row>
+    <row r="376">
+      <c r="A376" s="3"/>
+      <c r="B376" s="3"/>
+    </row>
+    <row r="377">
+      <c r="A377" s="3"/>
+      <c r="B377" s="3"/>
+    </row>
+    <row r="378">
+      <c r="A378" s="3"/>
+      <c r="B378" s="3"/>
+    </row>
+    <row r="379">
+      <c r="A379" s="3"/>
+      <c r="B379" s="3"/>
+    </row>
+    <row r="380">
+      <c r="A380" s="3"/>
+      <c r="B380" s="3"/>
+    </row>
+    <row r="381">
+      <c r="A381" s="3"/>
+      <c r="B381" s="3"/>
+    </row>
+    <row r="382">
+      <c r="A382" s="3"/>
+      <c r="B382" s="3"/>
+    </row>
+    <row r="383">
+      <c r="A383" s="3"/>
+      <c r="B383" s="3"/>
+    </row>
+    <row r="384">
+      <c r="A384" s="3"/>
+      <c r="B384" s="3"/>
+    </row>
+    <row r="385">
+      <c r="A385" s="3"/>
+      <c r="B385" s="3"/>
+    </row>
+    <row r="386">
+      <c r="A386" s="3"/>
+      <c r="B386" s="3"/>
+    </row>
+    <row r="387">
+      <c r="A387" s="3"/>
+      <c r="B387" s="3"/>
+    </row>
+    <row r="388">
+      <c r="A388" s="3"/>
+      <c r="B388" s="3"/>
+    </row>
+    <row r="389">
+      <c r="A389" s="3"/>
+      <c r="B389" s="3"/>
+    </row>
+    <row r="390">
+      <c r="A390" s="3"/>
+      <c r="B390" s="3"/>
+    </row>
+    <row r="391">
+      <c r="A391" s="3"/>
+      <c r="B391" s="3"/>
+    </row>
+    <row r="392">
+      <c r="A392" s="3"/>
+      <c r="B392" s="3"/>
+    </row>
+    <row r="393">
+      <c r="A393" s="3"/>
+      <c r="B393" s="3"/>
+    </row>
+    <row r="394">
+      <c r="A394" s="3"/>
+      <c r="B394" s="3"/>
+    </row>
+    <row r="395">
+      <c r="A395" s="3"/>
+      <c r="B395" s="3"/>
+    </row>
+    <row r="396">
+      <c r="A396" s="3"/>
+      <c r="B396" s="3"/>
+    </row>
+    <row r="397">
+      <c r="A397" s="3"/>
+      <c r="B397" s="3"/>
+    </row>
+    <row r="398">
+      <c r="A398" s="3"/>
+      <c r="B398" s="3"/>
+    </row>
+    <row r="399">
+      <c r="A399" s="3"/>
+      <c r="B399" s="3"/>
+    </row>
+    <row r="400">
+      <c r="A400" s="3"/>
+      <c r="B400" s="3"/>
+    </row>
+    <row r="401">
+      <c r="A401" s="3"/>
+      <c r="B401" s="3"/>
+    </row>
+    <row r="402">
+      <c r="A402" s="3"/>
+      <c r="B402" s="3"/>
+    </row>
+    <row r="403">
+      <c r="A403" s="3"/>
+      <c r="B403" s="3"/>
+    </row>
+    <row r="404">
+      <c r="A404" s="3"/>
+      <c r="B404" s="3"/>
+    </row>
+    <row r="405">
+      <c r="A405" s="3"/>
+      <c r="B405" s="3"/>
+    </row>
+    <row r="406">
+      <c r="A406" s="3"/>
+      <c r="B406" s="3"/>
+    </row>
+    <row r="407">
+      <c r="A407" s="3"/>
+      <c r="B407" s="3"/>
+    </row>
+    <row r="408">
+      <c r="A408" s="3"/>
+      <c r="B408" s="3"/>
+    </row>
+    <row r="409">
+      <c r="A409" s="3"/>
+      <c r="B409" s="3"/>
+    </row>
+    <row r="410">
+      <c r="A410" s="3"/>
+      <c r="B410" s="3"/>
+    </row>
+    <row r="411">
+      <c r="A411" s="3"/>
+      <c r="B411" s="3"/>
+    </row>
+    <row r="412">
+      <c r="A412" s="3"/>
+      <c r="B412" s="3"/>
+    </row>
+    <row r="413">
+      <c r="A413" s="3"/>
+      <c r="B413" s="3"/>
+    </row>
+    <row r="414">
+      <c r="A414" s="3"/>
+      <c r="B414" s="3"/>
+    </row>
+    <row r="415">
+      <c r="A415" s="3"/>
+      <c r="B415" s="3"/>
+    </row>
+    <row r="416">
+      <c r="A416" s="3"/>
+      <c r="B416" s="3"/>
+    </row>
+    <row r="417">
+      <c r="A417" s="3"/>
+      <c r="B417" s="3"/>
+    </row>
+    <row r="418">
+      <c r="A418" s="3"/>
+      <c r="B418" s="3"/>
+    </row>
+    <row r="419">
+      <c r="A419" s="3"/>
+      <c r="B419" s="3"/>
+    </row>
+    <row r="420">
+      <c r="A420" s="3"/>
+      <c r="B420" s="3"/>
+    </row>
+    <row r="421">
+      <c r="A421" s="3"/>
+      <c r="B421" s="3"/>
+    </row>
+    <row r="422">
+      <c r="A422" s="3"/>
+      <c r="B422" s="3"/>
+    </row>
+    <row r="423">
+      <c r="A423" s="3"/>
+      <c r="B423" s="3"/>
+    </row>
+    <row r="424">
+      <c r="A424" s="3"/>
+      <c r="B424" s="3"/>
+    </row>
+    <row r="425">
+      <c r="A425" s="3"/>
+      <c r="B425" s="3"/>
+    </row>
+    <row r="426">
+      <c r="A426" s="3"/>
+      <c r="B426" s="3"/>
+    </row>
+    <row r="427">
+      <c r="A427" s="3"/>
+      <c r="B427" s="3"/>
+    </row>
+    <row r="428">
+      <c r="A428" s="3"/>
+      <c r="B428" s="3"/>
+    </row>
+    <row r="429">
+      <c r="A429" s="3"/>
+      <c r="B429" s="3"/>
+    </row>
+    <row r="430">
+      <c r="A430" s="3"/>
+      <c r="B430" s="3"/>
+    </row>
+    <row r="431">
+      <c r="A431" s="3"/>
+      <c r="B431" s="3"/>
+    </row>
+    <row r="432">
+      <c r="A432" s="3"/>
+      <c r="B432" s="3"/>
+    </row>
+    <row r="433">
+      <c r="A433" s="3"/>
+      <c r="B433" s="3"/>
+    </row>
+    <row r="434">
+      <c r="A434" s="3"/>
+      <c r="B434" s="3"/>
+    </row>
+    <row r="435">
+      <c r="A435" s="3"/>
+      <c r="B435" s="3"/>
+    </row>
+    <row r="436">
+      <c r="A436" s="3"/>
+      <c r="B436" s="3"/>
+    </row>
+    <row r="437">
+      <c r="A437" s="3"/>
+      <c r="B437" s="3"/>
+    </row>
+    <row r="438">
+      <c r="A438" s="3"/>
+      <c r="B438" s="3"/>
+    </row>
+    <row r="439">
+      <c r="A439" s="3"/>
+      <c r="B439" s="3"/>
+    </row>
+    <row r="440">
+      <c r="A440" s="3"/>
+      <c r="B440" s="3"/>
+    </row>
+    <row r="441">
+      <c r="A441" s="3"/>
+      <c r="B441" s="3"/>
+    </row>
+    <row r="442">
+      <c r="A442" s="3"/>
+      <c r="B442" s="3"/>
+    </row>
+    <row r="443">
+      <c r="A443" s="3"/>
+      <c r="B443" s="3"/>
+    </row>
+    <row r="444">
+      <c r="A444" s="3"/>
+      <c r="B444" s="3"/>
+    </row>
+    <row r="445">
+      <c r="A445" s="3"/>
+      <c r="B445" s="3"/>
+    </row>
+    <row r="446">
+      <c r="A446" s="3"/>
+      <c r="B446" s="3"/>
+    </row>
+    <row r="447">
+      <c r="A447" s="3"/>
+      <c r="B447" s="3"/>
+    </row>
+    <row r="448">
+      <c r="A448" s="3"/>
+      <c r="B448" s="3"/>
+    </row>
+    <row r="449">
+      <c r="A449" s="3"/>
+      <c r="B449" s="3"/>
+    </row>
+    <row r="450">
+      <c r="A450" s="3"/>
+      <c r="B450" s="3"/>
+    </row>
+    <row r="451">
+      <c r="A451" s="3"/>
+      <c r="B451" s="3"/>
+    </row>
+    <row r="452">
+      <c r="A452" s="3"/>
+      <c r="B452" s="3"/>
+    </row>
+    <row r="453">
+      <c r="A453" s="3"/>
+      <c r="B453" s="3"/>
+    </row>
+    <row r="454">
+      <c r="A454" s="3"/>
+      <c r="B454" s="3"/>
+    </row>
+    <row r="455">
+      <c r="A455" s="3"/>
+      <c r="B455" s="3"/>
+    </row>
+    <row r="456">
+      <c r="A456" s="3"/>
+      <c r="B456" s="3"/>
+    </row>
+    <row r="457">
+      <c r="A457" s="3"/>
+      <c r="B457" s="3"/>
+    </row>
+    <row r="458">
+      <c r="A458" s="3"/>
+      <c r="B458" s="3"/>
+    </row>
+    <row r="459">
+      <c r="A459" s="3"/>
+      <c r="B459" s="3"/>
+    </row>
+    <row r="460">
+      <c r="A460" s="3"/>
+      <c r="B460" s="3"/>
+    </row>
+    <row r="461">
+      <c r="A461" s="3"/>
+      <c r="B461" s="3"/>
+    </row>
+    <row r="462">
+      <c r="A462" s="3"/>
+      <c r="B462" s="3"/>
+    </row>
+    <row r="463">
+      <c r="A463" s="3"/>
+      <c r="B463" s="3"/>
+    </row>
+    <row r="464">
+      <c r="A464" s="3"/>
+      <c r="B464" s="3"/>
+    </row>
+    <row r="465">
+      <c r="A465" s="3"/>
+      <c r="B465" s="3"/>
+    </row>
+    <row r="466">
+      <c r="A466" s="3"/>
+      <c r="B466" s="3"/>
+    </row>
+    <row r="467">
+      <c r="A467" s="3"/>
+      <c r="B467" s="3"/>
+    </row>
+    <row r="468">
+      <c r="A468" s="3"/>
+      <c r="B468" s="3"/>
+    </row>
+    <row r="469">
+      <c r="A469" s="3"/>
+      <c r="B469" s="3"/>
+    </row>
+    <row r="470">
+      <c r="A470" s="3"/>
+      <c r="B470" s="3"/>
+    </row>
+    <row r="471">
+      <c r="A471" s="3"/>
+      <c r="B471" s="3"/>
+    </row>
+    <row r="472">
+      <c r="A472" s="3"/>
+      <c r="B472" s="3"/>
+    </row>
+    <row r="473">
+      <c r="A473" s="3"/>
+      <c r="B473" s="3"/>
+    </row>
+    <row r="474">
+      <c r="A474" s="3"/>
+      <c r="B474" s="3"/>
+    </row>
+    <row r="475">
+      <c r="A475" s="3"/>
+      <c r="B475" s="3"/>
+    </row>
+    <row r="476">
+      <c r="A476" s="3"/>
+      <c r="B476" s="3"/>
+    </row>
+    <row r="477">
+      <c r="A477" s="3"/>
+      <c r="B477" s="3"/>
+    </row>
+    <row r="478">
+      <c r="A478" s="3"/>
+      <c r="B478" s="3"/>
+    </row>
+    <row r="479">
+      <c r="A479" s="3"/>
+      <c r="B479" s="3"/>
+    </row>
+    <row r="480">
+      <c r="A480" s="3"/>
+      <c r="B480" s="3"/>
+    </row>
+    <row r="481">
+      <c r="A481" s="3"/>
+      <c r="B481" s="3"/>
+    </row>
+    <row r="482">
+      <c r="A482" s="3"/>
+      <c r="B482" s="3"/>
+    </row>
+    <row r="483">
+      <c r="A483" s="3"/>
+      <c r="B483" s="3"/>
+    </row>
+    <row r="484">
+      <c r="A484" s="3"/>
+      <c r="B484" s="3"/>
+    </row>
+    <row r="485">
+      <c r="A485" s="3"/>
+      <c r="B485" s="3"/>
+    </row>
+    <row r="486">
+      <c r="A486" s="3"/>
+      <c r="B486" s="3"/>
+    </row>
+    <row r="487">
+      <c r="A487" s="3"/>
+      <c r="B487" s="3"/>
+    </row>
+    <row r="488">
+      <c r="A488" s="3"/>
+      <c r="B488" s="3"/>
+    </row>
+    <row r="489">
+      <c r="A489" s="3"/>
+      <c r="B489" s="3"/>
+    </row>
+    <row r="490">
+      <c r="A490" s="3"/>
+      <c r="B490" s="3"/>
+    </row>
+    <row r="491">
+      <c r="A491" s="3"/>
+      <c r="B491" s="3"/>
+    </row>
+    <row r="492">
+      <c r="A492" s="3"/>
+      <c r="B492" s="3"/>
+    </row>
+    <row r="493">
+      <c r="A493" s="3"/>
+      <c r="B493" s="3"/>
+    </row>
+    <row r="494">
+      <c r="A494" s="3"/>
+      <c r="B494" s="3"/>
+    </row>
+    <row r="495">
+      <c r="A495" s="3"/>
+      <c r="B495" s="3"/>
+    </row>
+    <row r="496">
+      <c r="A496" s="3"/>
+      <c r="B496" s="3"/>
+    </row>
+    <row r="497">
+      <c r="A497" s="3"/>
+      <c r="B497" s="3"/>
+    </row>
+    <row r="498">
+      <c r="A498" s="3"/>
+      <c r="B498" s="3"/>
+    </row>
+    <row r="499">
+      <c r="A499" s="3"/>
+      <c r="B499" s="3"/>
+    </row>
+    <row r="500">
+      <c r="A500" s="3"/>
+      <c r="B500" s="3"/>
+    </row>
+    <row r="501">
+      <c r="A501" s="3"/>
+      <c r="B501" s="3"/>
+    </row>
+    <row r="502">
+      <c r="A502" s="3"/>
+      <c r="B502" s="3"/>
+    </row>
+    <row r="503">
+      <c r="A503" s="3"/>
+      <c r="B503" s="3"/>
+    </row>
+    <row r="504">
+      <c r="A504" s="3"/>
+      <c r="B504" s="3"/>
+    </row>
+    <row r="505">
+      <c r="A505" s="3"/>
+      <c r="B505" s="3"/>
+    </row>
+    <row r="506">
+      <c r="A506" s="3"/>
+      <c r="B506" s="3"/>
+    </row>
+    <row r="507">
+      <c r="A507" s="3"/>
+      <c r="B507" s="3"/>
+    </row>
+    <row r="508">
+      <c r="A508" s="3"/>
+      <c r="B508" s="3"/>
+    </row>
+    <row r="509">
+      <c r="A509" s="3"/>
+      <c r="B509" s="3"/>
+    </row>
+    <row r="510">
+      <c r="A510" s="3"/>
+      <c r="B510" s="3"/>
+    </row>
+    <row r="511">
+      <c r="A511" s="3"/>
+      <c r="B511" s="3"/>
+    </row>
+    <row r="512">
+      <c r="A512" s="3"/>
+      <c r="B512" s="3"/>
+    </row>
+    <row r="513">
+      <c r="A513" s="3"/>
+      <c r="B513" s="3"/>
+    </row>
+    <row r="514">
+      <c r="A514" s="3"/>
+      <c r="B514" s="3"/>
+    </row>
+    <row r="515">
+      <c r="A515" s="3"/>
+      <c r="B515" s="3"/>
+    </row>
+    <row r="516">
+      <c r="A516" s="3"/>
+      <c r="B516" s="3"/>
+    </row>
+    <row r="517">
+      <c r="A517" s="3"/>
+      <c r="B517" s="3"/>
+    </row>
+    <row r="518">
+      <c r="A518" s="3"/>
+      <c r="B518" s="3"/>
+    </row>
+    <row r="519">
+      <c r="A519" s="3"/>
+      <c r="B519" s="3"/>
+    </row>
+    <row r="520">
+      <c r="A520" s="3"/>
+      <c r="B520" s="3"/>
+    </row>
+    <row r="521">
+      <c r="A521" s="3"/>
+      <c r="B521" s="3"/>
+    </row>
+    <row r="522">
+      <c r="A522" s="3"/>
+      <c r="B522" s="3"/>
+    </row>
+    <row r="523">
+      <c r="A523" s="3"/>
+      <c r="B523" s="3"/>
+    </row>
+    <row r="524">
+      <c r="A524" s="3"/>
+      <c r="B524" s="3"/>
+    </row>
+    <row r="525">
+      <c r="A525" s="3"/>
+      <c r="B525" s="3"/>
+    </row>
+    <row r="526">
+      <c r="A526" s="3"/>
+      <c r="B526" s="3"/>
+    </row>
+    <row r="527">
+      <c r="A527" s="3"/>
+      <c r="B527" s="3"/>
+    </row>
+    <row r="528">
+      <c r="A528" s="3"/>
+      <c r="B528" s="3"/>
+    </row>
+    <row r="529">
+      <c r="A529" s="3"/>
+      <c r="B529" s="3"/>
+    </row>
+    <row r="530">
+      <c r="A530" s="3"/>
+      <c r="B530" s="3"/>
+    </row>
+    <row r="531">
+      <c r="A531" s="3"/>
+      <c r="B531" s="3"/>
+    </row>
+    <row r="532">
+      <c r="A532" s="3"/>
+      <c r="B532" s="3"/>
+    </row>
+    <row r="533">
+      <c r="A533" s="3"/>
+      <c r="B533" s="3"/>
+    </row>
+    <row r="534">
+      <c r="A534" s="3"/>
+      <c r="B534" s="3"/>
+    </row>
+    <row r="535">
+      <c r="A535" s="3"/>
+      <c r="B535" s="3"/>
+    </row>
+    <row r="536">
+      <c r="A536" s="3"/>
+      <c r="B536" s="3"/>
+    </row>
+    <row r="537">
+      <c r="A537" s="3"/>
+      <c r="B537" s="3"/>
+    </row>
+    <row r="538">
+      <c r="A538" s="3"/>
+      <c r="B538" s="3"/>
+    </row>
+    <row r="539">
+      <c r="A539" s="3"/>
+      <c r="B539" s="3"/>
+    </row>
+    <row r="540">
+      <c r="A540" s="3"/>
+      <c r="B540" s="3"/>
+    </row>
+    <row r="541">
+      <c r="A541" s="3"/>
+      <c r="B541" s="3"/>
+    </row>
+    <row r="542">
+      <c r="A542" s="3"/>
+      <c r="B542" s="3"/>
+    </row>
+    <row r="543">
+      <c r="A543" s="3"/>
+      <c r="B543" s="3"/>
+    </row>
+    <row r="544">
+      <c r="A544" s="3"/>
+      <c r="B544" s="3"/>
+    </row>
+    <row r="545">
+      <c r="A545" s="3"/>
+      <c r="B545" s="3"/>
+    </row>
+    <row r="546">
+      <c r="A546" s="3"/>
+      <c r="B546" s="3"/>
+    </row>
+    <row r="547">
+      <c r="A547" s="3"/>
+      <c r="B547" s="3"/>
+    </row>
+    <row r="548">
+      <c r="A548" s="3"/>
+      <c r="B548" s="3"/>
+    </row>
+    <row r="549">
+      <c r="A549" s="3"/>
+      <c r="B549" s="3"/>
+    </row>
+    <row r="550">
+      <c r="A550" s="3"/>
+      <c r="B550" s="3"/>
+    </row>
+    <row r="551">
+      <c r="A551" s="3"/>
+      <c r="B551" s="3"/>
+    </row>
+    <row r="552">
+      <c r="A552" s="3"/>
+      <c r="B552" s="3"/>
+    </row>
+    <row r="553">
+      <c r="A553" s="3"/>
+      <c r="B553" s="3"/>
+    </row>
+    <row r="554">
+      <c r="A554" s="3"/>
+      <c r="B554" s="3"/>
+    </row>
+    <row r="555">
+      <c r="A555" s="3"/>
+      <c r="B555" s="3"/>
+    </row>
+    <row r="556">
+      <c r="A556" s="3"/>
+      <c r="B556" s="3"/>
+    </row>
+    <row r="557">
+      <c r="A557" s="3"/>
+      <c r="B557" s="3"/>
+    </row>
+    <row r="558">
+      <c r="A558" s="3"/>
+      <c r="B558" s="3"/>
+    </row>
+    <row r="559">
+      <c r="A559" s="3"/>
+      <c r="B559" s="3"/>
+    </row>
+    <row r="560">
+      <c r="A560" s="3"/>
+      <c r="B560" s="3"/>
+    </row>
+    <row r="561">
+      <c r="A561" s="3"/>
+      <c r="B561" s="3"/>
+    </row>
+    <row r="562">
+      <c r="A562" s="3"/>
+      <c r="B562" s="3"/>
+    </row>
+    <row r="563">
+      <c r="A563" s="3"/>
+      <c r="B563" s="3"/>
+    </row>
+    <row r="564">
+      <c r="A564" s="3"/>
+      <c r="B564" s="3"/>
+    </row>
+    <row r="565">
+      <c r="A565" s="3"/>
+      <c r="B565" s="3"/>
+    </row>
+    <row r="566">
+      <c r="A566" s="3"/>
+      <c r="B566" s="3"/>
+    </row>
+    <row r="567">
+      <c r="A567" s="3"/>
+      <c r="B567" s="3"/>
+    </row>
+    <row r="568">
+      <c r="A568" s="3"/>
+      <c r="B568" s="3"/>
+    </row>
+    <row r="569">
+      <c r="A569" s="3"/>
+      <c r="B569" s="3"/>
+    </row>
+    <row r="570">
+      <c r="A570" s="3"/>
+      <c r="B570" s="3"/>
+    </row>
+    <row r="571">
+      <c r="A571" s="3"/>
+      <c r="B571" s="3"/>
+    </row>
+    <row r="572">
+      <c r="A572" s="3"/>
+      <c r="B572" s="3"/>
+    </row>
+    <row r="573">
+      <c r="A573" s="3"/>
+      <c r="B573" s="3"/>
+    </row>
+    <row r="574">
+      <c r="A574" s="3"/>
+      <c r="B574" s="3"/>
+    </row>
+    <row r="575">
+      <c r="A575" s="3"/>
+      <c r="B575" s="3"/>
+    </row>
+    <row r="576">
+      <c r="A576" s="3"/>
+      <c r="B576" s="3"/>
+    </row>
+    <row r="577">
+      <c r="A577" s="3"/>
+      <c r="B577" s="3"/>
+    </row>
+    <row r="578">
+      <c r="A578" s="3"/>
+      <c r="B578" s="3"/>
+    </row>
+    <row r="579">
+      <c r="A579" s="3"/>
+      <c r="B579" s="3"/>
+    </row>
+    <row r="580">
+      <c r="A580" s="3"/>
+      <c r="B580" s="3"/>
+    </row>
+    <row r="581">
+      <c r="A581" s="3"/>
+      <c r="B581" s="3"/>
+    </row>
+    <row r="582">
+      <c r="A582" s="3"/>
+      <c r="B582" s="3"/>
+    </row>
+    <row r="583">
+      <c r="A583" s="3"/>
+      <c r="B583" s="3"/>
+    </row>
+    <row r="584">
+      <c r="A584" s="3"/>
+      <c r="B584" s="3"/>
+    </row>
+    <row r="585">
+      <c r="A585" s="3"/>
+      <c r="B585" s="3"/>
+    </row>
+    <row r="586">
+      <c r="A586" s="3"/>
+      <c r="B586" s="3"/>
+    </row>
+    <row r="587">
+      <c r="A587" s="3"/>
+      <c r="B587" s="3"/>
+    </row>
+    <row r="588">
+      <c r="A588" s="3"/>
+      <c r="B588" s="3"/>
+    </row>
+    <row r="589">
+      <c r="A589" s="3"/>
+      <c r="B589" s="3"/>
+    </row>
+    <row r="590">
+      <c r="A590" s="3"/>
+      <c r="B590" s="3"/>
+    </row>
+    <row r="591">
+      <c r="A591" s="3"/>
+      <c r="B591" s="3"/>
+    </row>
+    <row r="592">
+      <c r="A592" s="3"/>
+      <c r="B592" s="3"/>
+    </row>
+    <row r="593">
+      <c r="A593" s="3"/>
+      <c r="B593" s="3"/>
+    </row>
+    <row r="594">
+      <c r="A594" s="3"/>
+      <c r="B594" s="3"/>
+    </row>
+    <row r="595">
+      <c r="A595" s="3"/>
+      <c r="B595" s="3"/>
+    </row>
+    <row r="596">
+      <c r="A596" s="3"/>
+      <c r="B596" s="3"/>
+    </row>
+    <row r="597">
+      <c r="A597" s="3"/>
+      <c r="B597" s="3"/>
+    </row>
+    <row r="598">
+      <c r="A598" s="3"/>
+      <c r="B598" s="3"/>
+    </row>
+    <row r="599">
+      <c r="A599" s="3"/>
+      <c r="B599" s="3"/>
+    </row>
+    <row r="600">
+      <c r="A600" s="3"/>
+      <c r="B600" s="3"/>
+    </row>
+    <row r="601">
+      <c r="A601" s="3"/>
+      <c r="B601" s="3"/>
+    </row>
+    <row r="602">
+      <c r="A602" s="3"/>
+      <c r="B602" s="3"/>
+    </row>
+    <row r="603">
+      <c r="A603" s="3"/>
+      <c r="B603" s="3"/>
+    </row>
+    <row r="604">
+      <c r="A604" s="3"/>
+      <c r="B604" s="3"/>
+    </row>
+    <row r="605">
+      <c r="A605" s="3"/>
+      <c r="B605" s="3"/>
+    </row>
+    <row r="606">
+      <c r="A606" s="3"/>
+      <c r="B606" s="3"/>
+    </row>
+    <row r="607">
+      <c r="A607" s="3"/>
+      <c r="B607" s="3"/>
+    </row>
+    <row r="608">
+      <c r="A608" s="3"/>
+      <c r="B608" s="3"/>
+    </row>
+    <row r="609">
+      <c r="A609" s="3"/>
+      <c r="B609" s="3"/>
+    </row>
+    <row r="610">
+      <c r="A610" s="3"/>
+      <c r="B610" s="3"/>
+    </row>
+    <row r="611">
+      <c r="A611" s="3"/>
+      <c r="B611" s="3"/>
+    </row>
+    <row r="612">
+      <c r="A612" s="3"/>
+      <c r="B612" s="3"/>
+    </row>
+    <row r="613">
+      <c r="A613" s="3"/>
+      <c r="B613" s="3"/>
+    </row>
+    <row r="614">
+      <c r="A614" s="3"/>
+      <c r="B614" s="3"/>
+    </row>
+    <row r="615">
+      <c r="A615" s="3"/>
+      <c r="B615" s="3"/>
+    </row>
+    <row r="616">
+      <c r="A616" s="3"/>
+      <c r="B616" s="3"/>
+    </row>
+    <row r="617">
+      <c r="A617" s="3"/>
+      <c r="B617" s="3"/>
+    </row>
+    <row r="618">
+      <c r="A618" s="3"/>
+      <c r="B618" s="3"/>
+    </row>
+    <row r="619">
+      <c r="A619" s="3"/>
+      <c r="B619" s="3"/>
+    </row>
+    <row r="620">
+      <c r="A620" s="3"/>
+      <c r="B620" s="3"/>
+    </row>
+    <row r="621">
+      <c r="A621" s="3"/>
+      <c r="B621" s="3"/>
+    </row>
+    <row r="622">
+      <c r="A622" s="3"/>
+      <c r="B622" s="3"/>
+    </row>
+    <row r="623">
+      <c r="A623" s="3"/>
+      <c r="B623" s="3"/>
+    </row>
+    <row r="624">
+      <c r="A624" s="3"/>
+      <c r="B624" s="3"/>
+    </row>
+    <row r="625">
+      <c r="A625" s="3"/>
+      <c r="B625" s="3"/>
+    </row>
+    <row r="626">
+      <c r="A626" s="3"/>
+      <c r="B626" s="3"/>
+    </row>
+    <row r="627">
+      <c r="A627" s="3"/>
+      <c r="B627" s="3"/>
+    </row>
+    <row r="628">
+      <c r="A628" s="3"/>
+      <c r="B628" s="3"/>
+    </row>
+    <row r="629">
+      <c r="A629" s="3"/>
+      <c r="B629" s="3"/>
+    </row>
+    <row r="630">
+      <c r="A630" s="3"/>
+      <c r="B630" s="3"/>
+    </row>
+    <row r="631">
+      <c r="A631" s="3"/>
+      <c r="B631" s="3"/>
+    </row>
+    <row r="632">
+      <c r="A632" s="3"/>
+      <c r="B632" s="3"/>
+    </row>
+    <row r="633">
+      <c r="A633" s="3"/>
+      <c r="B633" s="3"/>
+    </row>
+    <row r="634">
+      <c r="A634" s="3"/>
+      <c r="B634" s="3"/>
+    </row>
+    <row r="635">
+      <c r="A635" s="3"/>
+      <c r="B635" s="3"/>
+    </row>
+    <row r="636">
+      <c r="A636" s="3"/>
+      <c r="B636" s="3"/>
+    </row>
+    <row r="637">
+      <c r="A637" s="3"/>
+      <c r="B637" s="3"/>
+    </row>
+    <row r="638">
+      <c r="A638" s="3"/>
+      <c r="B638" s="3"/>
+    </row>
+    <row r="639">
+      <c r="A639" s="3"/>
+      <c r="B639" s="3"/>
+    </row>
+    <row r="640">
+      <c r="A640" s="3"/>
+      <c r="B640" s="3"/>
+    </row>
+    <row r="641">
+      <c r="A641" s="3"/>
+      <c r="B641" s="3"/>
+    </row>
+    <row r="642">
+      <c r="A642" s="3"/>
+      <c r="B642" s="3"/>
+    </row>
+    <row r="643">
+      <c r="A643" s="3"/>
+      <c r="B643" s="3"/>
+    </row>
+    <row r="644">
+      <c r="A644" s="3"/>
+      <c r="B644" s="3"/>
+    </row>
+    <row r="645">
+      <c r="A645" s="3"/>
+      <c r="B645" s="3"/>
+    </row>
+    <row r="646">
+      <c r="A646" s="3"/>
+      <c r="B646" s="3"/>
+    </row>
+    <row r="647">
+      <c r="A647" s="3"/>
+      <c r="B647" s="3"/>
+    </row>
+    <row r="648">
+      <c r="A648" s="3"/>
+      <c r="B648" s="3"/>
+    </row>
+    <row r="649">
+      <c r="A649" s="3"/>
+      <c r="B649" s="3"/>
+    </row>
+    <row r="650">
+      <c r="A650" s="3"/>
+      <c r="B650" s="3"/>
+    </row>
+    <row r="651">
+      <c r="A651" s="3"/>
+      <c r="B651" s="3"/>
+    </row>
+    <row r="652">
+      <c r="A652" s="3"/>
+      <c r="B652" s="3"/>
+    </row>
+    <row r="653">
+      <c r="A653" s="3"/>
+      <c r="B653" s="3"/>
+    </row>
+    <row r="654">
+      <c r="A654" s="3"/>
+      <c r="B654" s="3"/>
+    </row>
+    <row r="655">
+      <c r="A655" s="3"/>
+      <c r="B655" s="3"/>
+    </row>
+    <row r="656">
+      <c r="A656" s="3"/>
+      <c r="B656" s="3"/>
+    </row>
+    <row r="657">
+      <c r="A657" s="3"/>
+      <c r="B657" s="3"/>
+    </row>
+    <row r="658">
+      <c r="A658" s="3"/>
+      <c r="B658" s="3"/>
+    </row>
+    <row r="659">
+      <c r="A659" s="3"/>
+      <c r="B659" s="3"/>
+    </row>
+    <row r="660">
+      <c r="A660" s="3"/>
+      <c r="B660" s="3"/>
+    </row>
+    <row r="661">
+      <c r="A661" s="3"/>
+      <c r="B661" s="3"/>
+    </row>
+    <row r="662">
+      <c r="A662" s="3"/>
+      <c r="B662" s="3"/>
+    </row>
+    <row r="663">
+      <c r="A663" s="3"/>
+      <c r="B663" s="3"/>
+    </row>
+    <row r="664">
+      <c r="A664" s="3"/>
+      <c r="B664" s="3"/>
+    </row>
+    <row r="665">
+      <c r="A665" s="3"/>
+      <c r="B665" s="3"/>
+    </row>
+    <row r="666">
+      <c r="A666" s="3"/>
+      <c r="B666" s="3"/>
+    </row>
+    <row r="667">
+      <c r="A667" s="3"/>
+      <c r="B667" s="3"/>
+    </row>
+    <row r="668">
+      <c r="A668" s="3"/>
+      <c r="B668" s="3"/>
+    </row>
+    <row r="669">
+      <c r="A669" s="3"/>
+      <c r="B669" s="3"/>
+    </row>
+    <row r="670">
+      <c r="A670" s="3"/>
+      <c r="B670" s="3"/>
+    </row>
+    <row r="671">
+      <c r="A671" s="3"/>
+      <c r="B671" s="3"/>
+    </row>
+    <row r="672">
+      <c r="A672" s="3"/>
+      <c r="B672" s="3"/>
+    </row>
+    <row r="673">
+      <c r="A673" s="3"/>
+      <c r="B673" s="3"/>
+    </row>
+    <row r="674">
+      <c r="A674" s="3"/>
+      <c r="B674" s="3"/>
+    </row>
+    <row r="675">
+      <c r="A675" s="3"/>
+      <c r="B675" s="3"/>
+    </row>
+    <row r="676">
+      <c r="A676" s="3"/>
+      <c r="B676" s="3"/>
+    </row>
+    <row r="677">
+      <c r="A677" s="3"/>
+      <c r="B677" s="3"/>
+    </row>
+    <row r="678">
+      <c r="A678" s="3"/>
+      <c r="B678" s="3"/>
+    </row>
+    <row r="679">
+      <c r="A679" s="3"/>
+      <c r="B679" s="3"/>
+    </row>
+    <row r="680">
+      <c r="A680" s="3"/>
+      <c r="B680" s="3"/>
+    </row>
+    <row r="681">
+      <c r="A681" s="3"/>
+      <c r="B681" s="3"/>
+    </row>
+    <row r="682">
+      <c r="A682" s="3"/>
+      <c r="B682" s="3"/>
+    </row>
+    <row r="683">
+      <c r="A683" s="3"/>
+      <c r="B683" s="3"/>
+    </row>
+    <row r="684">
+      <c r="A684" s="3"/>
+      <c r="B684" s="3"/>
+    </row>
+    <row r="685">
+      <c r="A685" s="3"/>
+      <c r="B685" s="3"/>
+    </row>
+    <row r="686">
+      <c r="A686" s="3"/>
+      <c r="B686" s="3"/>
+    </row>
+    <row r="687">
+      <c r="A687" s="3"/>
+      <c r="B687" s="3"/>
+    </row>
+    <row r="688">
+      <c r="A688" s="3"/>
+      <c r="B688" s="3"/>
+    </row>
+    <row r="689">
+      <c r="A689" s="3"/>
+      <c r="B689" s="3"/>
+    </row>
+    <row r="690">
+      <c r="A690" s="3"/>
+      <c r="B690" s="3"/>
+    </row>
+    <row r="691">
+      <c r="A691" s="3"/>
+      <c r="B691" s="3"/>
+    </row>
+    <row r="692">
+      <c r="A692" s="3"/>
+      <c r="B692" s="3"/>
+    </row>
+    <row r="693">
+      <c r="A693" s="3"/>
+      <c r="B693" s="3"/>
+    </row>
+    <row r="694">
+      <c r="A694" s="3"/>
+      <c r="B694" s="3"/>
+    </row>
+    <row r="695">
+      <c r="A695" s="3"/>
+      <c r="B695" s="3"/>
+    </row>
+    <row r="696">
+      <c r="A696" s="3"/>
+      <c r="B696" s="3"/>
+    </row>
+    <row r="697">
+      <c r="A697" s="3"/>
+      <c r="B697" s="3"/>
+    </row>
+    <row r="698">
+      <c r="A698" s="3"/>
+      <c r="B698" s="3"/>
+    </row>
+    <row r="699">
+      <c r="A699" s="3"/>
+      <c r="B699" s="3"/>
+    </row>
+    <row r="700">
+      <c r="A700" s="3"/>
+      <c r="B700" s="3"/>
+    </row>
+    <row r="701">
+      <c r="A701" s="3"/>
+      <c r="B701" s="3"/>
+    </row>
+    <row r="702">
+      <c r="A702" s="3"/>
+      <c r="B702" s="3"/>
+    </row>
+    <row r="703">
+      <c r="A703" s="3"/>
+      <c r="B703" s="3"/>
+    </row>
+    <row r="704">
+      <c r="A704" s="3"/>
+      <c r="B704" s="3"/>
+    </row>
+    <row r="705">
+      <c r="A705" s="3"/>
+      <c r="B705" s="3"/>
+    </row>
+    <row r="706">
+      <c r="A706" s="3"/>
+      <c r="B706" s="3"/>
+    </row>
+    <row r="707">
+      <c r="A707" s="3"/>
+      <c r="B707" s="3"/>
+    </row>
+    <row r="708">
+      <c r="A708" s="3"/>
+      <c r="B708" s="3"/>
+    </row>
+    <row r="709">
+      <c r="A709" s="3"/>
+      <c r="B709" s="3"/>
+    </row>
+    <row r="710">
+      <c r="A710" s="3"/>
+      <c r="B710" s="3"/>
+    </row>
+    <row r="711">
+      <c r="A711" s="3"/>
+      <c r="B711" s="3"/>
+    </row>
+    <row r="712">
+      <c r="A712" s="3"/>
+      <c r="B712" s="3"/>
+    </row>
+    <row r="713">
+      <c r="A713" s="3"/>
+      <c r="B713" s="3"/>
+    </row>
+    <row r="714">
+      <c r="A714" s="3"/>
+      <c r="B714" s="3"/>
+    </row>
+    <row r="715">
+      <c r="A715" s="3"/>
+      <c r="B715" s="3"/>
+    </row>
+    <row r="716">
+      <c r="A716" s="3"/>
+      <c r="B716" s="3"/>
+    </row>
+    <row r="717">
+      <c r="A717" s="3"/>
+      <c r="B717" s="3"/>
+    </row>
+    <row r="718">
+      <c r="A718" s="3"/>
+      <c r="B718" s="3"/>
+    </row>
+    <row r="719">
+      <c r="A719" s="3"/>
+      <c r="B719" s="3"/>
+    </row>
+    <row r="720">
+      <c r="A720" s="3"/>
+      <c r="B720" s="3"/>
+    </row>
+    <row r="721">
+      <c r="A721" s="3"/>
+      <c r="B721" s="3"/>
+    </row>
+    <row r="722">
+      <c r="A722" s="3"/>
+      <c r="B722" s="3"/>
+    </row>
+    <row r="723">
+      <c r="A723" s="3"/>
+      <c r="B723" s="3"/>
+    </row>
+    <row r="724">
+      <c r="A724" s="3"/>
+      <c r="B724" s="3"/>
+    </row>
+    <row r="725">
+      <c r="A725" s="3"/>
+      <c r="B725" s="3"/>
+    </row>
+    <row r="726">
+      <c r="A726" s="3"/>
+      <c r="B726" s="3"/>
+    </row>
+    <row r="727">
+      <c r="A727" s="3"/>
+      <c r="B727" s="3"/>
+    </row>
+    <row r="728">
+      <c r="A728" s="3"/>
+      <c r="B728" s="3"/>
+    </row>
+    <row r="729">
+      <c r="A729" s="3"/>
+      <c r="B729" s="3"/>
+    </row>
+    <row r="730">
+      <c r="A730" s="3"/>
+      <c r="B730" s="3"/>
+    </row>
+    <row r="731">
+      <c r="A731" s="3"/>
+      <c r="B731" s="3"/>
+    </row>
+    <row r="732">
+      <c r="A732" s="3"/>
+      <c r="B732" s="3"/>
+    </row>
+    <row r="733">
+      <c r="A733" s="3"/>
+      <c r="B733" s="3"/>
+    </row>
+    <row r="734">
+      <c r="A734" s="3"/>
+      <c r="B734" s="3"/>
+    </row>
+    <row r="735">
+      <c r="A735" s="3"/>
+      <c r="B735" s="3"/>
+    </row>
+    <row r="736">
+      <c r="A736" s="3"/>
+      <c r="B736" s="3"/>
+    </row>
+    <row r="737">
+      <c r="A737" s="3"/>
+      <c r="B737" s="3"/>
+    </row>
+    <row r="738">
+      <c r="A738" s="3"/>
+      <c r="B738" s="3"/>
+    </row>
+    <row r="739">
+      <c r="A739" s="3"/>
+      <c r="B739" s="3"/>
+    </row>
+    <row r="740">
+      <c r="A740" s="3"/>
+      <c r="B740" s="3"/>
+    </row>
+    <row r="741">
+      <c r="A741" s="3"/>
+      <c r="B741" s="3"/>
+    </row>
+    <row r="742">
+      <c r="A742" s="3"/>
+      <c r="B742" s="3"/>
+    </row>
+    <row r="743">
+      <c r="A743" s="3"/>
+      <c r="B743" s="3"/>
+    </row>
+    <row r="744">
+      <c r="A744" s="3"/>
+      <c r="B744" s="3"/>
+    </row>
+    <row r="745">
+      <c r="A745" s="3"/>
+      <c r="B745" s="3"/>
+    </row>
+    <row r="746">
+      <c r="A746" s="3"/>
+      <c r="B746" s="3"/>
+    </row>
+    <row r="747">
+      <c r="A747" s="3"/>
+      <c r="B747" s="3"/>
+    </row>
+    <row r="748">
+      <c r="A748" s="3"/>
+      <c r="B748" s="3"/>
+    </row>
+    <row r="749">
+      <c r="A749" s="3"/>
+      <c r="B749" s="3"/>
+    </row>
+    <row r="750">
+      <c r="A750" s="3"/>
+      <c r="B750" s="3"/>
+    </row>
+    <row r="751">
+      <c r="A751" s="3"/>
+      <c r="B751" s="3"/>
+    </row>
+    <row r="752">
+      <c r="A752" s="3"/>
+      <c r="B752" s="3"/>
+    </row>
+    <row r="753">
+      <c r="A753" s="3"/>
+      <c r="B753" s="3"/>
+    </row>
+    <row r="754">
+      <c r="A754" s="3"/>
+      <c r="B754" s="3"/>
+    </row>
+    <row r="755">
+      <c r="A755" s="3"/>
+      <c r="B755" s="3"/>
+    </row>
+    <row r="756">
+      <c r="A756" s="3"/>
+      <c r="B756" s="3"/>
+    </row>
+    <row r="757">
+      <c r="A757" s="3"/>
+      <c r="B757" s="3"/>
+    </row>
+    <row r="758">
+      <c r="A758" s="3"/>
+      <c r="B758" s="3"/>
+    </row>
+    <row r="759">
+      <c r="A759" s="3"/>
+      <c r="B759" s="3"/>
+    </row>
+    <row r="760">
+      <c r="A760" s="3"/>
+      <c r="B760" s="3"/>
+    </row>
+    <row r="761">
+      <c r="A761" s="3"/>
+      <c r="B761" s="3"/>
+    </row>
+    <row r="762">
+      <c r="A762" s="3"/>
+      <c r="B762" s="3"/>
+    </row>
+    <row r="763">
+      <c r="A763" s="3"/>
+      <c r="B763" s="3"/>
+    </row>
+    <row r="764">
+      <c r="A764" s="3"/>
+      <c r="B764" s="3"/>
+    </row>
+    <row r="765">
+      <c r="A765" s="3"/>
+      <c r="B765" s="3"/>
+    </row>
+    <row r="766">
+      <c r="A766" s="3"/>
+      <c r="B766" s="3"/>
+    </row>
+    <row r="767">
+      <c r="A767" s="3"/>
+      <c r="B767" s="3"/>
+    </row>
+    <row r="768">
+      <c r="A768" s="3"/>
+      <c r="B768" s="3"/>
+    </row>
+    <row r="769">
+      <c r="A769" s="3"/>
+      <c r="B769" s="3"/>
+    </row>
+    <row r="770">
+      <c r="A770" s="3"/>
+      <c r="B770" s="3"/>
+    </row>
+    <row r="771">
+      <c r="A771" s="3"/>
+      <c r="B771" s="3"/>
+    </row>
+    <row r="772">
+      <c r="A772" s="3"/>
+      <c r="B772" s="3"/>
+    </row>
+    <row r="773">
+      <c r="A773" s="3"/>
+      <c r="B773" s="3"/>
+    </row>
+    <row r="774">
+      <c r="A774" s="3"/>
+      <c r="B774" s="3"/>
+    </row>
+    <row r="775">
+      <c r="A775" s="3"/>
+      <c r="B775" s="3"/>
+    </row>
+    <row r="776">
+      <c r="A776" s="3"/>
+      <c r="B776" s="3"/>
+    </row>
+    <row r="777">
+      <c r="A777" s="3"/>
+      <c r="B777" s="3"/>
+    </row>
+    <row r="778">
+      <c r="A778" s="3"/>
+      <c r="B778" s="3"/>
+    </row>
+    <row r="779">
+      <c r="A779" s="3"/>
+      <c r="B779" s="3"/>
+    </row>
+    <row r="780">
+      <c r="A780" s="3"/>
+      <c r="B780" s="3"/>
+    </row>
+    <row r="781">
+      <c r="A781" s="3"/>
+      <c r="B781" s="3"/>
+    </row>
+    <row r="782">
+      <c r="A782" s="3"/>
+      <c r="B782" s="3"/>
+    </row>
+    <row r="783">
+      <c r="A783" s="3"/>
+      <c r="B783" s="3"/>
+    </row>
+    <row r="784">
+      <c r="A784" s="3"/>
+      <c r="B784" s="3"/>
+    </row>
+    <row r="785">
+      <c r="A785" s="3"/>
+      <c r="B785" s="3"/>
+    </row>
+    <row r="786">
+      <c r="A786" s="3"/>
+      <c r="B786" s="3"/>
+    </row>
+    <row r="787">
+      <c r="A787" s="3"/>
+      <c r="B787" s="3"/>
+    </row>
+    <row r="788">
+      <c r="A788" s="3"/>
+      <c r="B788" s="3"/>
+    </row>
+    <row r="789">
+      <c r="A789" s="3"/>
+      <c r="B789" s="3"/>
+    </row>
+    <row r="790">
+      <c r="A790" s="3"/>
+      <c r="B790" s="3"/>
+    </row>
+    <row r="791">
+      <c r="A791" s="3"/>
+      <c r="B791" s="3"/>
+    </row>
+    <row r="792">
+      <c r="A792" s="3"/>
+      <c r="B792" s="3"/>
+    </row>
+    <row r="793">
+      <c r="A793" s="3"/>
+      <c r="B793" s="3"/>
+    </row>
+    <row r="794">
+      <c r="A794" s="3"/>
+      <c r="B794" s="3"/>
+    </row>
+    <row r="795">
+      <c r="A795" s="3"/>
+      <c r="B795" s="3"/>
+    </row>
+    <row r="796">
+      <c r="A796" s="3"/>
+      <c r="B796" s="3"/>
+    </row>
+    <row r="797">
+      <c r="A797" s="3"/>
+      <c r="B797" s="3"/>
+    </row>
+    <row r="798">
+      <c r="A798" s="3"/>
+      <c r="B798" s="3"/>
+    </row>
+    <row r="799">
+      <c r="A799" s="3"/>
+      <c r="B799" s="3"/>
+    </row>
+    <row r="800">
+      <c r="A800" s="3"/>
+      <c r="B800" s="3"/>
+    </row>
+    <row r="801">
+      <c r="A801" s="3"/>
+      <c r="B801" s="3"/>
+    </row>
+    <row r="802">
+      <c r="A802" s="3"/>
+      <c r="B802" s="3"/>
+    </row>
+    <row r="803">
+      <c r="A803" s="3"/>
+      <c r="B803" s="3"/>
+    </row>
+    <row r="804">
+      <c r="A804" s="3"/>
+      <c r="B804" s="3"/>
+    </row>
+    <row r="805">
+      <c r="A805" s="3"/>
+      <c r="B805" s="3"/>
+    </row>
+    <row r="806">
+      <c r="A806" s="3"/>
+      <c r="B806" s="3"/>
+    </row>
+    <row r="807">
+      <c r="A807" s="3"/>
+      <c r="B807" s="3"/>
+    </row>
+    <row r="808">
+      <c r="A808" s="3"/>
+      <c r="B808" s="3"/>
+    </row>
+    <row r="809">
+      <c r="A809" s="3"/>
+      <c r="B809" s="3"/>
+    </row>
+    <row r="810">
+      <c r="A810" s="3"/>
+      <c r="B810" s="3"/>
+    </row>
+    <row r="811">
+      <c r="A811" s="3"/>
+      <c r="B811" s="3"/>
+    </row>
+    <row r="812">
+      <c r="A812" s="3"/>
+      <c r="B812" s="3"/>
+    </row>
+    <row r="813">
+      <c r="A813" s="3"/>
+      <c r="B813" s="3"/>
+    </row>
+    <row r="814">
+      <c r="A814" s="3"/>
+      <c r="B814" s="3"/>
+    </row>
+    <row r="815">
+      <c r="A815" s="3"/>
+      <c r="B815" s="3"/>
+    </row>
+    <row r="816">
+      <c r="A816" s="3"/>
+      <c r="B816" s="3"/>
+    </row>
+    <row r="817">
+      <c r="A817" s="3"/>
+      <c r="B817" s="3"/>
+    </row>
+    <row r="818">
+      <c r="A818" s="3"/>
+      <c r="B818" s="3"/>
+    </row>
+    <row r="819">
+      <c r="A819" s="3"/>
+      <c r="B819" s="3"/>
+    </row>
+    <row r="820">
+      <c r="A820" s="3"/>
+      <c r="B820" s="3"/>
+    </row>
+    <row r="821">
+      <c r="A821" s="3"/>
+      <c r="B821" s="3"/>
+    </row>
+    <row r="822">
+      <c r="A822" s="3"/>
+      <c r="B822" s="3"/>
+    </row>
+    <row r="823">
+      <c r="A823" s="3"/>
+      <c r="B823" s="3"/>
+    </row>
+    <row r="824">
+      <c r="A824" s="3"/>
+      <c r="B824" s="3"/>
+    </row>
+    <row r="825">
+      <c r="A825" s="3"/>
+      <c r="B825" s="3"/>
+    </row>
+    <row r="826">
+      <c r="A826" s="3"/>
+      <c r="B826" s="3"/>
+    </row>
+    <row r="827">
+      <c r="A827" s="3"/>
+      <c r="B827" s="3"/>
+    </row>
+    <row r="828">
+      <c r="A828" s="3"/>
+      <c r="B828" s="3"/>
+    </row>
+    <row r="829">
+      <c r="A829" s="3"/>
+      <c r="B829" s="3"/>
+    </row>
+    <row r="830">
+      <c r="A830" s="3"/>
+      <c r="B830" s="3"/>
+    </row>
+    <row r="831">
+      <c r="A831" s="3"/>
+      <c r="B831" s="3"/>
+    </row>
+    <row r="832">
+      <c r="A832" s="3"/>
+      <c r="B832" s="3"/>
+    </row>
+    <row r="833">
+      <c r="A833" s="3"/>
+      <c r="B833" s="3"/>
+    </row>
+    <row r="834">
+      <c r="A834" s="3"/>
+      <c r="B834" s="3"/>
+    </row>
+    <row r="835">
+      <c r="A835" s="3"/>
+      <c r="B835" s="3"/>
+    </row>
+    <row r="836">
+      <c r="A836" s="3"/>
+      <c r="B836" s="3"/>
+    </row>
+    <row r="837">
+      <c r="A837" s="3"/>
+      <c r="B837" s="3"/>
+    </row>
+    <row r="838">
+      <c r="A838" s="3"/>
+      <c r="B838" s="3"/>
+    </row>
+    <row r="839">
+      <c r="A839" s="3"/>
+      <c r="B839" s="3"/>
+    </row>
+    <row r="840">
+      <c r="A840" s="3"/>
+      <c r="B840" s="3"/>
+    </row>
+    <row r="841">
+      <c r="A841" s="3"/>
+      <c r="B841" s="3"/>
+    </row>
+    <row r="842">
+      <c r="A842" s="3"/>
+      <c r="B842" s="3"/>
+    </row>
+    <row r="843">
+      <c r="A843" s="3"/>
+      <c r="B843" s="3"/>
+    </row>
+    <row r="844">
+      <c r="A844" s="3"/>
+      <c r="B844" s="3"/>
+    </row>
+    <row r="845">
+      <c r="A845" s="3"/>
+      <c r="B845" s="3"/>
+    </row>
+    <row r="846">
+      <c r="A846" s="3"/>
+      <c r="B846" s="3"/>
+    </row>
+    <row r="847">
+      <c r="A847" s="3"/>
+      <c r="B847" s="3"/>
+    </row>
+    <row r="848">
+      <c r="A848" s="3"/>
+      <c r="B848" s="3"/>
+    </row>
+    <row r="849">
+      <c r="A849" s="3"/>
+      <c r="B849" s="3"/>
+    </row>
+    <row r="850">
+      <c r="A850" s="3"/>
+      <c r="B850" s="3"/>
+    </row>
+    <row r="851">
+      <c r="A851" s="3"/>
+      <c r="B851" s="3"/>
+    </row>
+    <row r="852">
+      <c r="A852" s="3"/>
+      <c r="B852" s="3"/>
+    </row>
+    <row r="853">
+      <c r="A853" s="3"/>
+      <c r="B853" s="3"/>
+    </row>
+    <row r="854">
+      <c r="A854" s="3"/>
+      <c r="B854" s="3"/>
+    </row>
+    <row r="855">
+      <c r="A855" s="3"/>
+      <c r="B855" s="3"/>
+    </row>
+    <row r="856">
+      <c r="A856" s="3"/>
+      <c r="B856" s="3"/>
+    </row>
+    <row r="857">
+      <c r="A857" s="3"/>
+      <c r="B857" s="3"/>
+    </row>
+    <row r="858">
+      <c r="A858" s="3"/>
+      <c r="B858" s="3"/>
+    </row>
+    <row r="859">
+      <c r="A859" s="3"/>
+      <c r="B859" s="3"/>
+    </row>
+    <row r="860">
+      <c r="A860" s="3"/>
+      <c r="B860" s="3"/>
+    </row>
+    <row r="861">
+      <c r="A861" s="3"/>
+      <c r="B861" s="3"/>
+    </row>
+    <row r="862">
+      <c r="A862" s="3"/>
+      <c r="B862" s="3"/>
+    </row>
+    <row r="863">
+      <c r="A863" s="3"/>
+      <c r="B863" s="3"/>
+    </row>
+    <row r="864">
+      <c r="A864" s="3"/>
+      <c r="B864" s="3"/>
+    </row>
+    <row r="865">
+      <c r="A865" s="3"/>
+      <c r="B865" s="3"/>
+    </row>
+    <row r="866">
+      <c r="A866" s="3"/>
+      <c r="B866" s="3"/>
+    </row>
+    <row r="867">
+      <c r="A867" s="3"/>
+      <c r="B867" s="3"/>
+    </row>
+    <row r="868">
+      <c r="A868" s="3"/>
+      <c r="B868" s="3"/>
+    </row>
+    <row r="869">
+      <c r="A869" s="3"/>
+      <c r="B869" s="3"/>
+    </row>
+    <row r="870">
+      <c r="A870" s="3"/>
+      <c r="B870" s="3"/>
+    </row>
+    <row r="871">
+      <c r="A871" s="3"/>
+      <c r="B871" s="3"/>
+    </row>
+    <row r="872">
+      <c r="A872" s="3"/>
+      <c r="B872" s="3"/>
+    </row>
+    <row r="873">
+      <c r="A873" s="3"/>
+      <c r="B873" s="3"/>
+    </row>
+    <row r="874">
+      <c r="A874" s="3"/>
+      <c r="B874" s="3"/>
+    </row>
+    <row r="875">
+      <c r="A875" s="3"/>
+      <c r="B875" s="3"/>
+    </row>
+    <row r="876">
+      <c r="A876" s="3"/>
+      <c r="B876" s="3"/>
+    </row>
+    <row r="877">
+      <c r="A877" s="3"/>
+      <c r="B877" s="3"/>
+    </row>
+    <row r="878">
+      <c r="A878" s="3"/>
+      <c r="B878" s="3"/>
+    </row>
+    <row r="879">
+      <c r="A879" s="3"/>
+      <c r="B879" s="3"/>
+    </row>
+    <row r="880">
+      <c r="A880" s="3"/>
+      <c r="B880" s="3"/>
+    </row>
+    <row r="881">
+      <c r="A881" s="3"/>
+      <c r="B881" s="3"/>
+    </row>
+    <row r="882">
+      <c r="A882" s="3"/>
+      <c r="B882" s="3"/>
+    </row>
+    <row r="883">
+      <c r="A883" s="3"/>
+      <c r="B883" s="3"/>
+    </row>
+    <row r="884">
+      <c r="A884" s="3"/>
+      <c r="B884" s="3"/>
+    </row>
+    <row r="885">
+      <c r="A885" s="3"/>
+      <c r="B885" s="3"/>
+    </row>
+    <row r="886">
+      <c r="A886" s="3"/>
+      <c r="B886" s="3"/>
+    </row>
+    <row r="887">
+      <c r="A887" s="3"/>
+      <c r="B887" s="3"/>
+    </row>
+    <row r="888">
+      <c r="A888" s="3"/>
+      <c r="B888" s="3"/>
+    </row>
+    <row r="889">
+      <c r="A889" s="3"/>
+      <c r="B889" s="3"/>
+    </row>
+    <row r="890">
+      <c r="A890" s="3"/>
+      <c r="B890" s="3"/>
+    </row>
+    <row r="891">
+      <c r="A891" s="3"/>
+      <c r="B891" s="3"/>
+    </row>
+    <row r="892">
+      <c r="A892" s="3"/>
+      <c r="B892" s="3"/>
+    </row>
+    <row r="893">
+      <c r="A893" s="3"/>
+      <c r="B893" s="3"/>
+    </row>
+    <row r="894">
+      <c r="A894" s="3"/>
+      <c r="B894" s="3"/>
+    </row>
+    <row r="895">
+      <c r="A895" s="3"/>
+      <c r="B895" s="3"/>
+    </row>
+    <row r="896">
+      <c r="A896" s="3"/>
+      <c r="B896" s="3"/>
+    </row>
+    <row r="897">
+      <c r="A897" s="3"/>
+      <c r="B897" s="3"/>
+    </row>
+    <row r="898">
+      <c r="A898" s="3"/>
+      <c r="B898" s="3"/>
+    </row>
+    <row r="899">
+      <c r="A899" s="3"/>
+      <c r="B899" s="3"/>
+    </row>
+    <row r="900">
+      <c r="A900" s="3"/>
+      <c r="B900" s="3"/>
+    </row>
+    <row r="901">
+      <c r="A901" s="3"/>
+      <c r="B901" s="3"/>
+    </row>
+    <row r="902">
+      <c r="A902" s="3"/>
+      <c r="B902" s="3"/>
+    </row>
+    <row r="903">
+      <c r="A903" s="3"/>
+      <c r="B903" s="3"/>
+    </row>
+    <row r="904">
+      <c r="A904" s="3"/>
+      <c r="B904" s="3"/>
+    </row>
+    <row r="905">
+      <c r="A905" s="3"/>
+      <c r="B905" s="3"/>
+    </row>
+    <row r="906">
+      <c r="A906" s="3"/>
+      <c r="B906" s="3"/>
+    </row>
+    <row r="907">
+      <c r="A907" s="3"/>
+      <c r="B907" s="3"/>
+    </row>
+    <row r="908">
+      <c r="A908" s="3"/>
+      <c r="B908" s="3"/>
+    </row>
+    <row r="909">
+      <c r="A909" s="3"/>
+      <c r="B909" s="3"/>
+    </row>
+    <row r="910">
+      <c r="A910" s="3"/>
+      <c r="B910" s="3"/>
+    </row>
+    <row r="911">
+      <c r="A911" s="3"/>
+      <c r="B911" s="3"/>
+    </row>
+    <row r="912">
+      <c r="A912" s="3"/>
+      <c r="B912" s="3"/>
+    </row>
+    <row r="913">
+      <c r="A913" s="3"/>
+      <c r="B913" s="3"/>
+    </row>
+    <row r="914">
+      <c r="A914" s="3"/>
+      <c r="B914" s="3"/>
+    </row>
+    <row r="915">
+      <c r="A915" s="3"/>
+      <c r="B915" s="3"/>
+    </row>
+    <row r="916">
+      <c r="A916" s="3"/>
+      <c r="B916" s="3"/>
+    </row>
+    <row r="917">
+      <c r="A917" s="3"/>
+      <c r="B917" s="3"/>
+    </row>
+    <row r="918">
+      <c r="A918" s="3"/>
+      <c r="B918" s="3"/>
+    </row>
+    <row r="919">
+      <c r="A919" s="3"/>
+      <c r="B919" s="3"/>
+    </row>
+    <row r="920">
+      <c r="A920" s="3"/>
+      <c r="B920" s="3"/>
+    </row>
+    <row r="921">
+      <c r="A921" s="3"/>
+      <c r="B921" s="3"/>
+    </row>
+    <row r="922">
+      <c r="A922" s="3"/>
+      <c r="B922" s="3"/>
+    </row>
+    <row r="923">
+      <c r="A923" s="3"/>
+      <c r="B923" s="3"/>
+    </row>
+    <row r="924">
+      <c r="A924" s="3"/>
+      <c r="B924" s="3"/>
+    </row>
+    <row r="925">
+      <c r="A925" s="3"/>
+      <c r="B925" s="3"/>
+    </row>
+    <row r="926">
+      <c r="A926" s="3"/>
+      <c r="B926" s="3"/>
+    </row>
+    <row r="927">
+      <c r="A927" s="3"/>
+      <c r="B927" s="3"/>
+    </row>
+    <row r="928">
+      <c r="A928" s="3"/>
+      <c r="B928" s="3"/>
+    </row>
+    <row r="929">
+      <c r="A929" s="3"/>
+      <c r="B929" s="3"/>
+    </row>
+    <row r="930">
+      <c r="A930" s="3"/>
+      <c r="B930" s="3"/>
+    </row>
+    <row r="931">
+      <c r="A931" s="3"/>
+      <c r="B931" s="3"/>
+    </row>
+    <row r="932">
+      <c r="A932" s="3"/>
+      <c r="B932" s="3"/>
+    </row>
+    <row r="933">
+      <c r="A933" s="3"/>
+      <c r="B933" s="3"/>
+    </row>
+    <row r="934">
+      <c r="A934" s="3"/>
+      <c r="B934" s="3"/>
+    </row>
+    <row r="935">
+      <c r="A935" s="3"/>
+      <c r="B935" s="3"/>
+    </row>
+    <row r="936">
+      <c r="A936" s="3"/>
+      <c r="B936" s="3"/>
+    </row>
+    <row r="937">
+      <c r="A937" s="3"/>
+      <c r="B937" s="3"/>
+    </row>
+    <row r="938">
+      <c r="A938" s="3"/>
+      <c r="B938" s="3"/>
+    </row>
+    <row r="939">
+      <c r="A939" s="3"/>
+      <c r="B939" s="3"/>
+    </row>
+    <row r="940">
+      <c r="A940" s="3"/>
+      <c r="B940" s="3"/>
+    </row>
+    <row r="941">
+      <c r="A941" s="3"/>
+      <c r="B941" s="3"/>
+    </row>
+    <row r="942">
+      <c r="A942" s="3"/>
+      <c r="B942" s="3"/>
+    </row>
+    <row r="943">
+      <c r="A943" s="3"/>
+      <c r="B943" s="3"/>
+    </row>
+    <row r="944">
+      <c r="A944" s="3"/>
+      <c r="B944" s="3"/>
+    </row>
+    <row r="945">
+      <c r="A945" s="3"/>
+      <c r="B945" s="3"/>
+    </row>
+    <row r="946">
+      <c r="A946" s="3"/>
+      <c r="B946" s="3"/>
+    </row>
+    <row r="947">
+      <c r="A947" s="3"/>
+      <c r="B947" s="3"/>
+    </row>
+    <row r="948">
+      <c r="A948" s="3"/>
+      <c r="B948" s="3"/>
+    </row>
+    <row r="949">
+      <c r="A949" s="3"/>
+      <c r="B949" s="3"/>
+    </row>
+    <row r="950">
+      <c r="A950" s="3"/>
+      <c r="B950" s="3"/>
+    </row>
+    <row r="951">
+      <c r="A951" s="3"/>
+      <c r="B951" s="3"/>
+    </row>
+    <row r="952">
+      <c r="A952" s="3"/>
+      <c r="B952" s="3"/>
+    </row>
+    <row r="953">
+      <c r="A953" s="3"/>
+      <c r="B953" s="3"/>
+    </row>
+    <row r="954">
+      <c r="A954" s="3"/>
+      <c r="B954" s="3"/>
+    </row>
+    <row r="955">
+      <c r="A955" s="3"/>
+      <c r="B955" s="3"/>
+    </row>
+    <row r="956">
+      <c r="A956" s="3"/>
+      <c r="B956" s="3"/>
+    </row>
+    <row r="957">
+      <c r="A957" s="3"/>
+      <c r="B957" s="3"/>
+    </row>
+    <row r="958">
+      <c r="A958" s="3"/>
+      <c r="B958" s="3"/>
+    </row>
+    <row r="959">
+      <c r="A959" s="3"/>
+      <c r="B959" s="3"/>
+    </row>
+    <row r="960">
+      <c r="A960" s="3"/>
+      <c r="B960" s="3"/>
+    </row>
+    <row r="961">
+      <c r="A961" s="3"/>
+      <c r="B961" s="3"/>
+    </row>
+    <row r="962">
+      <c r="A962" s="3"/>
+      <c r="B962" s="3"/>
+    </row>
+    <row r="963">
+      <c r="A963" s="3"/>
+      <c r="B963" s="3"/>
+    </row>
+    <row r="964">
+      <c r="A964" s="3"/>
+      <c r="B964" s="3"/>
+    </row>
+    <row r="965">
+      <c r="A965" s="3"/>
+      <c r="B965" s="3"/>
+    </row>
+    <row r="966">
+      <c r="A966" s="3"/>
+      <c r="B966" s="3"/>
+    </row>
+    <row r="967">
+      <c r="A967" s="3"/>
+      <c r="B967" s="3"/>
+    </row>
+    <row r="968">
+      <c r="A968" s="3"/>
+      <c r="B968" s="3"/>
+    </row>
+    <row r="969">
+      <c r="A969" s="3"/>
+      <c r="B969" s="3"/>
+    </row>
+    <row r="970">
+      <c r="A970" s="3"/>
+      <c r="B970" s="3"/>
+    </row>
+    <row r="971">
+      <c r="A971" s="3"/>
+      <c r="B971" s="3"/>
+    </row>
+    <row r="972">
+      <c r="A972" s="3"/>
+      <c r="B972" s="3"/>
+    </row>
+    <row r="973">
+      <c r="A973" s="3"/>
+      <c r="B973" s="3"/>
+    </row>
+    <row r="974">
+      <c r="A974" s="3"/>
+      <c r="B974" s="3"/>
+    </row>
+    <row r="975">
+      <c r="A975" s="3"/>
+      <c r="B975" s="3"/>
+    </row>
+    <row r="976">
+      <c r="A976" s="3"/>
+      <c r="B976" s="3"/>
+    </row>
+    <row r="977">
+      <c r="A977" s="3"/>
+      <c r="B977" s="3"/>
+    </row>
+    <row r="978">
+      <c r="A978" s="3"/>
+      <c r="B978" s="3"/>
+    </row>
+    <row r="979">
+      <c r="A979" s="3"/>
+      <c r="B979" s="3"/>
+    </row>
+    <row r="980">
+      <c r="A980" s="3"/>
+      <c r="B980" s="3"/>
+    </row>
+    <row r="981">
+      <c r="A981" s="3"/>
+      <c r="B981" s="3"/>
+    </row>
+    <row r="982">
+      <c r="A982" s="3"/>
+      <c r="B982" s="3"/>
+    </row>
+    <row r="983">
+      <c r="A983" s="3"/>
+      <c r="B983" s="3"/>
+    </row>
+    <row r="984">
+      <c r="A984" s="3"/>
+      <c r="B984" s="3"/>
+    </row>
+    <row r="985">
+      <c r="A985" s="3"/>
+      <c r="B985" s="3"/>
+    </row>
+    <row r="986">
+      <c r="A986" s="3"/>
+      <c r="B986" s="3"/>
+    </row>
+    <row r="987">
+      <c r="A987" s="3"/>
+      <c r="B987" s="3"/>
+    </row>
+    <row r="988">
+      <c r="A988" s="3"/>
+      <c r="B988" s="3"/>
+    </row>
+    <row r="989">
+      <c r="A989" s="3"/>
+      <c r="B989" s="3"/>
+    </row>
+    <row r="990">
+      <c r="A990" s="3"/>
+      <c r="B990" s="3"/>
+    </row>
+    <row r="991">
+      <c r="A991" s="3"/>
+      <c r="B991" s="3"/>
+    </row>
+    <row r="992">
+      <c r="A992" s="3"/>
+      <c r="B992" s="3"/>
+    </row>
+    <row r="993">
+      <c r="A993" s="3"/>
+      <c r="B993" s="3"/>
+    </row>
+    <row r="994">
+      <c r="A994" s="3"/>
+      <c r="B994" s="3"/>
+    </row>
+    <row r="995">
+      <c r="A995" s="3"/>
+      <c r="B995" s="3"/>
+    </row>
+    <row r="996">
+      <c r="A996" s="3"/>
+      <c r="B996" s="3"/>
+    </row>
+    <row r="997">
+      <c r="A997" s="3"/>
+      <c r="B997" s="3"/>
+    </row>
+    <row r="998">
+      <c r="A998" s="3"/>
+      <c r="B998" s="3"/>
+    </row>
+    <row r="999">
+      <c r="A999" s="3"/>
+      <c r="B999" s="3"/>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>